<commit_message>
finalized all the benchmarks
</commit_message>
<xml_diff>
--- a/benchmarks/summary_ali.xlsx
+++ b/benchmarks/summary_ali.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -206,8 +206,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
   </fills>
@@ -308,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,7 +453,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -461,23 +481,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,51 +489,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -545,7 +505,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,10 +518,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,9 +545,9 @@
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J83" activeCellId="0" sqref="J83"/>
+      <selection pane="bottomLeft" activeCell="I66" activeCellId="0" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2872,10 +2832,7 @@
         <f aca="false">ROUND(2*E61*E64/(E61+E64),3)</f>
         <v>0.736</v>
       </c>
-      <c r="F58" s="12" t="e">
-        <f aca="false">ROUND(2*F61*F64/(F61+F64),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F58" s="35"/>
       <c r="G58" s="11" t="n">
         <f aca="false">ROUND(2*G61*G64/(G61+G64),3)</f>
         <v>0.632</v>
@@ -2915,10 +2872,7 @@
         <f aca="false">ROUND(2*E62*E65/(E62+E65),3)</f>
         <v>0.75</v>
       </c>
-      <c r="F59" s="18" t="e">
-        <f aca="false">ROUND(2*F62*F65/(F62+F65),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F59" s="36"/>
       <c r="G59" s="17" t="n">
         <f aca="false">ROUND(2*G62*G65/(G62+G65),3)</f>
         <v>0.624</v>
@@ -2958,10 +2912,7 @@
         <f aca="false">ROUND(2*E63*E66/(E63+E66),3)</f>
         <v>0.78</v>
       </c>
-      <c r="F60" s="21" t="e">
-        <f aca="false">ROUND(2*F63*F66/(F63+F66),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F60" s="37"/>
       <c r="G60" s="20" t="n">
         <f aca="false">ROUND(2*G63*G66/(G63+G66),3)</f>
         <v>0.699</v>
@@ -3002,7 +2953,7 @@
       <c r="E61" s="25" t="n">
         <v>0.761</v>
       </c>
-      <c r="F61" s="35"/>
+      <c r="F61" s="38"/>
       <c r="G61" s="23" t="n">
         <v>0.65</v>
       </c>
@@ -3012,13 +2963,13 @@
       <c r="I61" s="23" t="n">
         <v>0.6</v>
       </c>
-      <c r="J61" s="36" t="n">
+      <c r="J61" s="23" t="n">
         <v>0.614</v>
       </c>
-      <c r="K61" s="36" t="n">
+      <c r="K61" s="23" t="n">
         <v>0.634</v>
       </c>
-      <c r="L61" s="37" t="n">
+      <c r="L61" s="24" t="n">
         <v>0.589</v>
       </c>
       <c r="M61" s="14"/>
@@ -3036,7 +2987,7 @@
       <c r="E62" s="14" t="n">
         <v>0.754</v>
       </c>
-      <c r="F62" s="38"/>
+      <c r="F62" s="39"/>
       <c r="G62" s="14" t="n">
         <v>0.624</v>
       </c>
@@ -3046,13 +2997,13 @@
       <c r="I62" s="14" t="n">
         <v>0.601</v>
       </c>
-      <c r="J62" s="39" t="n">
+      <c r="J62" s="14" t="n">
         <v>0.563</v>
       </c>
-      <c r="K62" s="39" t="n">
+      <c r="K62" s="14" t="n">
         <v>0.711</v>
       </c>
-      <c r="L62" s="40" t="n">
+      <c r="L62" s="27" t="n">
         <v>0.533</v>
       </c>
       <c r="M62" s="14"/>
@@ -3068,7 +3019,7 @@
       <c r="E63" s="34" t="n">
         <v>0.767</v>
       </c>
-      <c r="F63" s="41"/>
+      <c r="F63" s="40"/>
       <c r="G63" s="28" t="n">
         <v>0.679</v>
       </c>
@@ -3078,13 +3029,13 @@
       <c r="I63" s="28" t="n">
         <v>0.599</v>
       </c>
-      <c r="J63" s="42" t="n">
+      <c r="J63" s="28" t="n">
         <v>0.675</v>
       </c>
-      <c r="K63" s="42" t="n">
+      <c r="K63" s="28" t="n">
         <v>0.573</v>
       </c>
-      <c r="L63" s="43" t="n">
+      <c r="L63" s="29" t="n">
         <v>0.659</v>
       </c>
       <c r="M63" s="14"/>
@@ -3105,7 +3056,7 @@
       <c r="E64" s="25" t="n">
         <v>0.713</v>
       </c>
-      <c r="F64" s="35"/>
+      <c r="F64" s="38"/>
       <c r="G64" s="23" t="n">
         <v>0.615</v>
       </c>
@@ -3115,13 +3066,13 @@
       <c r="I64" s="23" t="n">
         <v>0.569</v>
       </c>
-      <c r="J64" s="36" t="n">
+      <c r="J64" s="23" t="n">
         <v>0.59</v>
       </c>
-      <c r="K64" s="36" t="n">
+      <c r="K64" s="23" t="n">
         <v>0.583</v>
       </c>
-      <c r="L64" s="37" t="n">
+      <c r="L64" s="24" t="n">
         <v>0.57</v>
       </c>
       <c r="M64" s="14"/>
@@ -3137,7 +3088,7 @@
       <c r="E65" s="14" t="n">
         <v>0.746</v>
       </c>
-      <c r="F65" s="38"/>
+      <c r="F65" s="39"/>
       <c r="G65" s="14" t="n">
         <v>0.624</v>
       </c>
@@ -3147,13 +3098,13 @@
       <c r="I65" s="14" t="n">
         <v>0.577</v>
       </c>
-      <c r="J65" s="39" t="n">
+      <c r="J65" s="14" t="n">
         <v>0.566</v>
       </c>
-      <c r="K65" s="39" t="n">
+      <c r="K65" s="14" t="n">
         <v>0.648</v>
       </c>
-      <c r="L65" s="40" t="n">
+      <c r="L65" s="27" t="n">
         <v>0.539</v>
       </c>
       <c r="M65" s="14"/>
@@ -3169,7 +3120,7 @@
       <c r="E66" s="34" t="n">
         <v>0.793</v>
       </c>
-      <c r="F66" s="41"/>
+      <c r="F66" s="40"/>
       <c r="G66" s="28" t="n">
         <v>0.72</v>
       </c>
@@ -3179,13 +3130,13 @@
       <c r="I66" s="28" t="n">
         <v>0.677</v>
       </c>
-      <c r="J66" s="42" t="n">
+      <c r="J66" s="28" t="n">
         <v>0.735</v>
       </c>
-      <c r="K66" s="42" t="n">
+      <c r="K66" s="28" t="n">
         <v>0.652</v>
       </c>
-      <c r="L66" s="43" t="n">
+      <c r="L66" s="29" t="n">
         <v>0.724</v>
       </c>
       <c r="M66" s="14"/>
@@ -3202,7 +3153,7 @@
       <c r="E67" s="3" t="n">
         <v>212.5</v>
       </c>
-      <c r="F67" s="44"/>
+      <c r="F67" s="41"/>
       <c r="G67" s="3" t="n">
         <v>12000.2</v>
       </c>
@@ -3212,13 +3163,13 @@
       <c r="I67" s="3" t="n">
         <v>1482.4</v>
       </c>
-      <c r="J67" s="45" t="n">
+      <c r="J67" s="3" t="n">
         <v>28858.6</v>
       </c>
-      <c r="K67" s="45" t="n">
+      <c r="K67" s="3" t="n">
         <v>28777.5</v>
       </c>
-      <c r="L67" s="45" t="n">
+      <c r="L67" s="3" t="n">
         <v>28604.9</v>
       </c>
       <c r="M67" s="14"/>
@@ -3244,10 +3195,7 @@
         <f aca="false">ROUND(2*E71*E74/(E71+E74),3)</f>
         <v>0.79</v>
       </c>
-      <c r="F68" s="12" t="e">
-        <f aca="false">ROUND(2*F71*F74/(F71+F74),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F68" s="35"/>
       <c r="G68" s="11" t="n">
         <f aca="false">ROUND(2*G71*G74/(G71+G74),3)</f>
         <v>0.744</v>
@@ -3260,15 +3208,15 @@
         <f aca="false">ROUND(2*I71*I74/(I71+I74),3)</f>
         <v>0.769</v>
       </c>
-      <c r="J68" s="46" t="n">
+      <c r="J68" s="11" t="n">
         <f aca="false">ROUND(2*J71*J74/(J71+J74),3)</f>
         <v>0.779</v>
       </c>
-      <c r="K68" s="46" t="n">
+      <c r="K68" s="11" t="n">
         <f aca="false">ROUND(2*K71*K74/(K71+K74),3)</f>
         <v>0.784</v>
       </c>
-      <c r="L68" s="47" t="n">
+      <c r="L68" s="12" t="n">
         <f aca="false">ROUND(2*L71*L74/(L71+L74),3)</f>
         <v>0.769</v>
       </c>
@@ -3288,10 +3236,7 @@
         <f aca="false">ROUND(2*E72*E75/(E72+E75),3)</f>
         <v>0.899</v>
       </c>
-      <c r="F69" s="18" t="e">
-        <f aca="false">ROUND(2*F72*F75/(F72+F75),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F69" s="36"/>
       <c r="G69" s="17" t="n">
         <f aca="false">ROUND(2*G72*G75/(G72+G75),3)</f>
         <v>0.737</v>
@@ -3304,15 +3249,15 @@
         <f aca="false">ROUND(2*I72*I75/(I72+I75),3)</f>
         <v>0.77</v>
       </c>
-      <c r="J69" s="48" t="n">
+      <c r="J69" s="17" t="n">
         <f aca="false">ROUND(2*J72*J75/(J72+J75),3)</f>
         <v>0.741</v>
       </c>
-      <c r="K69" s="48" t="n">
+      <c r="K69" s="17" t="n">
         <f aca="false">ROUND(2*K72*K75/(K72+K75),3)</f>
         <v>0.82</v>
       </c>
-      <c r="L69" s="49" t="n">
+      <c r="L69" s="18" t="n">
         <f aca="false">ROUND(2*L72*L75/(L72+L75),3)</f>
         <v>0.722</v>
       </c>
@@ -3332,10 +3277,7 @@
         <f aca="false">ROUND(2*E73*E76/(E73+E76),3)</f>
         <v>0.731</v>
       </c>
-      <c r="F70" s="21" t="e">
-        <f aca="false">ROUND(2*F73*F76/(F73+F76),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F70" s="37"/>
       <c r="G70" s="20" t="n">
         <f aca="false">ROUND(2*G73*G76/(G73+G76),3)</f>
         <v>0.781</v>
@@ -3348,15 +3290,15 @@
         <f aca="false">ROUND(2*I73*I76/(I73+I76),3)</f>
         <v>0.789</v>
       </c>
-      <c r="J70" s="50" t="n">
+      <c r="J70" s="20" t="n">
         <f aca="false">ROUND(2*J73*J76/(J73+J76),3)</f>
         <v>0.845</v>
       </c>
-      <c r="K70" s="50" t="n">
+      <c r="K70" s="20" t="n">
         <f aca="false">ROUND(2*K73*K76/(K73+K76),3)</f>
         <v>0.772</v>
       </c>
-      <c r="L70" s="51" t="n">
+      <c r="L70" s="22" t="n">
         <f aca="false">ROUND(2*L73*L76/(L73+L76),3)</f>
         <v>0.847</v>
       </c>
@@ -3377,7 +3319,7 @@
       <c r="E71" s="23" t="n">
         <v>0.802</v>
       </c>
-      <c r="F71" s="35"/>
+      <c r="F71" s="38"/>
       <c r="G71" s="23" t="n">
         <v>0.747</v>
       </c>
@@ -3387,13 +3329,13 @@
       <c r="I71" s="23" t="n">
         <v>0.762</v>
       </c>
-      <c r="J71" s="36" t="n">
+      <c r="J71" s="23" t="n">
         <v>0.782</v>
       </c>
-      <c r="K71" s="36" t="n">
+      <c r="K71" s="23" t="n">
         <v>0.778</v>
       </c>
-      <c r="L71" s="37" t="n">
+      <c r="L71" s="24" t="n">
         <v>0.769</v>
       </c>
       <c r="M71" s="14"/>
@@ -3412,7 +3354,7 @@
       <c r="E72" s="14" t="n">
         <v>0.903</v>
       </c>
-      <c r="F72" s="38"/>
+      <c r="F72" s="39"/>
       <c r="G72" s="14" t="n">
         <v>0.728</v>
       </c>
@@ -3422,13 +3364,13 @@
       <c r="I72" s="14" t="n">
         <v>0.778</v>
       </c>
-      <c r="J72" s="39" t="n">
+      <c r="J72" s="14" t="n">
         <v>0.748</v>
       </c>
-      <c r="K72" s="39" t="n">
+      <c r="K72" s="14" t="n">
         <v>0.834</v>
       </c>
-      <c r="L72" s="40" t="n">
+      <c r="L72" s="27" t="n">
         <v>0.725</v>
       </c>
       <c r="M72" s="14"/>
@@ -3445,7 +3387,7 @@
       <c r="E73" s="28" t="n">
         <v>0.721</v>
       </c>
-      <c r="F73" s="41"/>
+      <c r="F73" s="40"/>
       <c r="G73" s="28" t="n">
         <v>0.767</v>
       </c>
@@ -3455,13 +3397,13 @@
       <c r="I73" s="28" t="n">
         <v>0.747</v>
       </c>
-      <c r="J73" s="52" t="n">
+      <c r="J73" s="34" t="n">
         <v>0.819</v>
       </c>
-      <c r="K73" s="42" t="n">
+      <c r="K73" s="28" t="n">
         <v>0.73</v>
       </c>
-      <c r="L73" s="53" t="n">
+      <c r="L73" s="30" t="n">
         <v>0.819</v>
       </c>
       <c r="M73" s="14"/>
@@ -3483,7 +3425,7 @@
       <c r="E74" s="23" t="n">
         <v>0.778</v>
       </c>
-      <c r="F74" s="35"/>
+      <c r="F74" s="38"/>
       <c r="G74" s="23" t="n">
         <v>0.741</v>
       </c>
@@ -3493,13 +3435,13 @@
       <c r="I74" s="23" t="n">
         <v>0.777</v>
       </c>
-      <c r="J74" s="36" t="n">
+      <c r="J74" s="23" t="n">
         <v>0.777</v>
       </c>
-      <c r="K74" s="54" t="n">
+      <c r="K74" s="25" t="n">
         <v>0.791</v>
       </c>
-      <c r="L74" s="37" t="n">
+      <c r="L74" s="24" t="n">
         <v>0.77</v>
       </c>
       <c r="M74" s="14"/>
@@ -3516,7 +3458,7 @@
       <c r="E75" s="14" t="n">
         <v>0.895</v>
       </c>
-      <c r="F75" s="38"/>
+      <c r="F75" s="39"/>
       <c r="G75" s="14" t="n">
         <v>0.746</v>
       </c>
@@ -3526,13 +3468,13 @@
       <c r="I75" s="14" t="n">
         <v>0.763</v>
       </c>
-      <c r="J75" s="39" t="n">
+      <c r="J75" s="14" t="n">
         <v>0.735</v>
       </c>
-      <c r="K75" s="39" t="n">
+      <c r="K75" s="14" t="n">
         <v>0.806</v>
       </c>
-      <c r="L75" s="40" t="n">
+      <c r="L75" s="27" t="n">
         <v>0.719</v>
       </c>
       <c r="M75" s="14"/>
@@ -3549,7 +3491,7 @@
       <c r="E76" s="28" t="n">
         <v>0.742</v>
       </c>
-      <c r="F76" s="41"/>
+      <c r="F76" s="40"/>
       <c r="G76" s="28" t="n">
         <v>0.796</v>
       </c>
@@ -3559,13 +3501,13 @@
       <c r="I76" s="28" t="n">
         <v>0.836</v>
       </c>
-      <c r="J76" s="42" t="n">
+      <c r="J76" s="28" t="n">
         <v>0.873</v>
       </c>
-      <c r="K76" s="42" t="n">
+      <c r="K76" s="28" t="n">
         <v>0.82</v>
       </c>
-      <c r="L76" s="53" t="n">
+      <c r="L76" s="30" t="n">
         <v>0.877</v>
       </c>
       <c r="M76" s="14"/>
@@ -3589,10 +3531,7 @@
         <f aca="false">ROUND(2*E80*E83/(E80+E83),3)</f>
         <v>0.802</v>
       </c>
-      <c r="F77" s="12" t="e">
-        <f aca="false">ROUND(2*F80*F83/(F80+F83),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F77" s="35"/>
       <c r="G77" s="11" t="n">
         <f aca="false">ROUND(2*G80*G83/(G80+G83),3)</f>
         <v>0.803</v>
@@ -3605,15 +3544,15 @@
         <f aca="false">ROUND(2*I80*I83/(I80+I83),3)</f>
         <v>0.848</v>
       </c>
-      <c r="J77" s="46" t="n">
+      <c r="J77" s="11" t="n">
         <f aca="false">ROUND(2*J80*J83/(J80+J83),3)</f>
         <v>0.846</v>
       </c>
-      <c r="K77" s="55" t="n">
+      <c r="K77" s="32" t="n">
         <f aca="false">ROUND(2*K80*K83/(K80+K83),3)</f>
         <v>0.862</v>
       </c>
-      <c r="L77" s="47" t="n">
+      <c r="L77" s="12" t="n">
         <f aca="false">ROUND(2*L80*L83/(L80+L83),3)</f>
         <v>0.84</v>
       </c>
@@ -3633,10 +3572,7 @@
         <f aca="false">ROUND(2*E81*E84/(E81+E84),3)</f>
         <v>0.95</v>
       </c>
-      <c r="F78" s="18" t="e">
-        <f aca="false">ROUND(2*F81*F84/(F81+F84),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F78" s="36"/>
       <c r="G78" s="17" t="n">
         <f aca="false">ROUND(2*G81*G84/(G81+G84),3)</f>
         <v>0.807</v>
@@ -3649,15 +3585,15 @@
         <f aca="false">ROUND(2*I81*I84/(I81+I84),3)</f>
         <v>0.847</v>
       </c>
-      <c r="J78" s="48" t="n">
+      <c r="J78" s="17" t="n">
         <f aca="false">ROUND(2*J81*J84/(J81+J84),3)</f>
         <v>0.826</v>
       </c>
-      <c r="K78" s="48" t="n">
+      <c r="K78" s="17" t="n">
         <f aca="false">ROUND(2*K81*K84/(K81+K84),3)</f>
         <v>0.889</v>
       </c>
-      <c r="L78" s="49" t="n">
+      <c r="L78" s="18" t="n">
         <f aca="false">ROUND(2*L81*L84/(L81+L84),3)</f>
         <v>0.809</v>
       </c>
@@ -3677,10 +3613,7 @@
         <f aca="false">ROUND(2*E82*E85/(E82+E85),3)</f>
         <v>0.709</v>
       </c>
-      <c r="F79" s="21" t="e">
-        <f aca="false">ROUND(2*F82*F85/(F82+F85),3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F79" s="37"/>
       <c r="G79" s="20" t="n">
         <f aca="false">ROUND(2*G82*G85/(G82+G85),3)</f>
         <v>0.823</v>
@@ -3693,15 +3626,15 @@
         <f aca="false">ROUND(2*I82*I85/(I82+I85),3)</f>
         <v>0.854</v>
       </c>
-      <c r="J79" s="50" t="n">
+      <c r="J79" s="20" t="n">
         <f aca="false">ROUND(2*J82*J85/(J82+J85),3)</f>
         <v>0.874</v>
       </c>
-      <c r="K79" s="50" t="n">
+      <c r="K79" s="20" t="n">
         <f aca="false">ROUND(2*K82*K85/(K82+K85),3)</f>
         <v>0.841</v>
       </c>
-      <c r="L79" s="51" t="n">
+      <c r="L79" s="22" t="n">
         <f aca="false">ROUND(2*L82*L85/(L82+L85),3)</f>
         <v>0.881</v>
       </c>
@@ -3722,7 +3655,7 @@
       <c r="E80" s="23" t="n">
         <v>0.797</v>
       </c>
-      <c r="F80" s="35"/>
+      <c r="F80" s="38"/>
       <c r="G80" s="23" t="n">
         <v>0.812</v>
       </c>
@@ -3732,13 +3665,13 @@
       <c r="I80" s="23" t="n">
         <v>0.858</v>
       </c>
-      <c r="J80" s="36" t="n">
+      <c r="J80" s="23" t="n">
         <v>0.857</v>
       </c>
-      <c r="K80" s="54" t="n">
+      <c r="K80" s="25" t="n">
         <v>0.869</v>
       </c>
-      <c r="L80" s="37" t="n">
+      <c r="L80" s="24" t="n">
         <v>0.85</v>
       </c>
       <c r="M80" s="14"/>
@@ -3757,7 +3690,7 @@
       <c r="E81" s="14" t="n">
         <v>0.947</v>
       </c>
-      <c r="F81" s="38"/>
+      <c r="F81" s="39"/>
       <c r="G81" s="14" t="n">
         <v>0.803</v>
       </c>
@@ -3767,13 +3700,13 @@
       <c r="I81" s="14" t="n">
         <v>0.86</v>
       </c>
-      <c r="J81" s="39" t="n">
+      <c r="J81" s="14" t="n">
         <v>0.836</v>
       </c>
-      <c r="K81" s="39" t="n">
+      <c r="K81" s="14" t="n">
         <v>0.9</v>
       </c>
-      <c r="L81" s="40" t="n">
+      <c r="L81" s="27" t="n">
         <v>0.818</v>
       </c>
       <c r="M81" s="14"/>
@@ -3790,7 +3723,7 @@
       <c r="E82" s="28" t="n">
         <v>0.688</v>
       </c>
-      <c r="F82" s="41"/>
+      <c r="F82" s="40"/>
       <c r="G82" s="28" t="n">
         <v>0.822</v>
       </c>
@@ -3800,13 +3733,13 @@
       <c r="I82" s="28" t="n">
         <v>0.855</v>
       </c>
-      <c r="J82" s="42" t="n">
+      <c r="J82" s="28" t="n">
         <v>0.879</v>
       </c>
-      <c r="K82" s="42" t="n">
+      <c r="K82" s="28" t="n">
         <v>0.841</v>
       </c>
-      <c r="L82" s="53" t="n">
+      <c r="L82" s="30" t="n">
         <v>0.884</v>
       </c>
       <c r="M82" s="14"/>
@@ -3828,7 +3761,7 @@
       <c r="E83" s="23" t="n">
         <v>0.807</v>
       </c>
-      <c r="F83" s="35"/>
+      <c r="F83" s="38"/>
       <c r="G83" s="23" t="n">
         <v>0.794</v>
       </c>
@@ -3838,13 +3771,13 @@
       <c r="I83" s="23" t="n">
         <v>0.839</v>
       </c>
-      <c r="J83" s="36" t="n">
+      <c r="J83" s="23" t="n">
         <v>0.836</v>
       </c>
-      <c r="K83" s="54" t="n">
+      <c r="K83" s="25" t="n">
         <v>0.855</v>
       </c>
-      <c r="L83" s="37" t="n">
+      <c r="L83" s="24" t="n">
         <v>0.831</v>
       </c>
       <c r="M83" s="14"/>
@@ -3861,7 +3794,7 @@
       <c r="E84" s="26" t="n">
         <v>0.954</v>
       </c>
-      <c r="F84" s="38"/>
+      <c r="F84" s="39"/>
       <c r="G84" s="14" t="n">
         <v>0.811</v>
       </c>
@@ -3871,13 +3804,13 @@
       <c r="I84" s="14" t="n">
         <v>0.835</v>
       </c>
-      <c r="J84" s="39" t="n">
+      <c r="J84" s="14" t="n">
         <v>0.816</v>
       </c>
-      <c r="K84" s="39" t="n">
+      <c r="K84" s="14" t="n">
         <v>0.879</v>
       </c>
-      <c r="L84" s="40" t="n">
+      <c r="L84" s="27" t="n">
         <v>0.801</v>
       </c>
       <c r="M84" s="14"/>
@@ -3894,7 +3827,7 @@
       <c r="E85" s="28" t="n">
         <v>0.732</v>
       </c>
-      <c r="F85" s="41"/>
+      <c r="F85" s="40"/>
       <c r="G85" s="28" t="n">
         <v>0.825</v>
       </c>
@@ -3904,13 +3837,13 @@
       <c r="I85" s="28" t="n">
         <v>0.854</v>
       </c>
-      <c r="J85" s="42" t="n">
+      <c r="J85" s="28" t="n">
         <v>0.87</v>
       </c>
-      <c r="K85" s="42" t="n">
+      <c r="K85" s="28" t="n">
         <v>0.842</v>
       </c>
-      <c r="L85" s="43" t="n">
+      <c r="L85" s="29" t="n">
         <v>0.878</v>
       </c>
       <c r="M85" s="14"/>
@@ -3934,9 +3867,9 @@
         <f aca="false">ROUND(2*E89*E92/(E89+E92),3)</f>
         <v>0.738</v>
       </c>
-      <c r="F86" s="12" t="e">
+      <c r="F86" s="12" t="n">
         <f aca="false">ROUND(2*F89*F92/(F89+F92),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.647</v>
       </c>
       <c r="G86" s="11" t="n">
         <f aca="false">ROUND(2*G89*G92/(G89+G92),3)</f>
@@ -3975,9 +3908,9 @@
         <f aca="false">ROUND(2*E90*E93/(E90+E93),3)</f>
         <v>0.871</v>
       </c>
-      <c r="F87" s="18" t="e">
+      <c r="F87" s="18" t="n">
         <f aca="false">ROUND(2*F90*F93/(F90+F93),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.78</v>
       </c>
       <c r="G87" s="17" t="n">
         <f aca="false">ROUND(2*G90*G93/(G90+G93),3)</f>
@@ -4016,9 +3949,9 @@
         <f aca="false">ROUND(2*E91*E94/(E91+E94),3)</f>
         <v>0.654</v>
       </c>
-      <c r="F88" s="21" t="e">
+      <c r="F88" s="21" t="n">
         <f aca="false">ROUND(2*F91*F94/(F91+F94),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.559</v>
       </c>
       <c r="G88" s="20" t="n">
         <f aca="false">ROUND(2*G91*G94/(G91+G94),3)</f>
@@ -4058,7 +3991,9 @@
       <c r="E89" s="23" t="n">
         <v>0.75</v>
       </c>
-      <c r="F89" s="35"/>
+      <c r="F89" s="42" t="n">
+        <v>0.657</v>
+      </c>
       <c r="G89" s="23" t="n">
         <v>0.58</v>
       </c>
@@ -4088,7 +4023,9 @@
       <c r="E90" s="14" t="n">
         <v>0.861</v>
       </c>
-      <c r="F90" s="38"/>
+      <c r="F90" s="43" t="n">
+        <v>0.784</v>
+      </c>
       <c r="G90" s="14" t="n">
         <v>0.599</v>
       </c>
@@ -4118,7 +4055,9 @@
       <c r="E91" s="28" t="n">
         <v>0.664</v>
       </c>
-      <c r="F91" s="41"/>
+      <c r="F91" s="44" t="n">
+        <v>0.566</v>
+      </c>
       <c r="G91" s="28" t="n">
         <v>0.562</v>
       </c>
@@ -4151,7 +4090,9 @@
       <c r="E92" s="23" t="n">
         <v>0.726</v>
       </c>
-      <c r="F92" s="35"/>
+      <c r="F92" s="42" t="n">
+        <v>0.638</v>
+      </c>
       <c r="G92" s="23" t="n">
         <v>0.615</v>
       </c>
@@ -4181,7 +4122,9 @@
       <c r="E93" s="14" t="n">
         <v>0.882</v>
       </c>
-      <c r="F93" s="38"/>
+      <c r="F93" s="43" t="n">
+        <v>0.777</v>
+      </c>
       <c r="G93" s="14" t="n">
         <v>0.642</v>
       </c>
@@ -4211,7 +4154,9 @@
       <c r="E94" s="28" t="n">
         <v>0.644</v>
       </c>
-      <c r="F94" s="41"/>
+      <c r="F94" s="44" t="n">
+        <v>0.553</v>
+      </c>
       <c r="G94" s="28" t="n">
         <v>0.604</v>
       </c>
@@ -4242,7 +4187,9 @@
       <c r="E95" s="3" t="n">
         <v>259.1</v>
       </c>
-      <c r="F95" s="44"/>
+      <c r="F95" s="45" t="n">
+        <v>86705.3</v>
+      </c>
       <c r="G95" s="3" t="n">
         <v>8483.4</v>
       </c>
@@ -4280,9 +4227,9 @@
         <f aca="false">ROUND(2*E99*E102/(E99+E102),3)</f>
         <v>0.753</v>
       </c>
-      <c r="F96" s="12" t="e">
+      <c r="F96" s="12" t="n">
         <f aca="false">ROUND(2*F99*F102/(F99+F102),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.665</v>
       </c>
       <c r="G96" s="11" t="n">
         <f aca="false">ROUND(2*G99*G102/(G99+G102),3)</f>
@@ -4322,9 +4269,9 @@
         <f aca="false">ROUND(2*E100*E103/(E100+E103),3)</f>
         <v>0.928</v>
       </c>
-      <c r="F97" s="18" t="e">
+      <c r="F97" s="18" t="n">
         <f aca="false">ROUND(2*F100*F103/(F100+F103),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.842</v>
       </c>
       <c r="G97" s="17" t="n">
         <f aca="false">ROUND(2*G100*G103/(G100+G103),3)</f>
@@ -4364,9 +4311,9 @@
         <f aca="false">ROUND(2*E101*E104/(E101+E104),3)</f>
         <v>0.647</v>
       </c>
-      <c r="F98" s="21" t="e">
+      <c r="F98" s="21" t="n">
         <f aca="false">ROUND(2*F101*F104/(F101+F104),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.551</v>
       </c>
       <c r="G98" s="20" t="n">
         <f aca="false">ROUND(2*G101*G104/(G101+G104),3)</f>
@@ -4407,7 +4354,9 @@
       <c r="E99" s="23" t="n">
         <v>0.763</v>
       </c>
-      <c r="F99" s="35"/>
+      <c r="F99" s="42" t="n">
+        <v>0.68</v>
+      </c>
       <c r="G99" s="23" t="n">
         <v>0.75</v>
       </c>
@@ -4438,7 +4387,9 @@
       <c r="E100" s="14" t="n">
         <v>0.924</v>
       </c>
-      <c r="F100" s="38"/>
+      <c r="F100" s="43" t="n">
+        <v>0.867</v>
+      </c>
       <c r="G100" s="14" t="n">
         <v>0.777</v>
       </c>
@@ -4469,7 +4420,9 @@
       <c r="E101" s="28" t="n">
         <v>0.65</v>
       </c>
-      <c r="F101" s="41"/>
+      <c r="F101" s="44" t="n">
+        <v>0.56</v>
+      </c>
       <c r="G101" s="28" t="n">
         <v>0.725</v>
       </c>
@@ -4503,7 +4456,9 @@
       <c r="E102" s="23" t="n">
         <v>0.743</v>
       </c>
-      <c r="F102" s="35"/>
+      <c r="F102" s="42" t="n">
+        <v>0.65</v>
+      </c>
       <c r="G102" s="23" t="n">
         <v>0.77</v>
       </c>
@@ -4534,7 +4489,9 @@
       <c r="E103" s="14" t="n">
         <v>0.932</v>
       </c>
-      <c r="F103" s="38"/>
+      <c r="F103" s="43" t="n">
+        <v>0.819</v>
+      </c>
       <c r="G103" s="14" t="n">
         <v>0.789</v>
       </c>
@@ -4565,7 +4522,9 @@
       <c r="E104" s="28" t="n">
         <v>0.644</v>
       </c>
-      <c r="F104" s="41"/>
+      <c r="F104" s="44" t="n">
+        <v>0.543</v>
+      </c>
       <c r="G104" s="28" t="n">
         <v>0.759</v>
       </c>
@@ -4774,10 +4733,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4786,7 +4745,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="4.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.47"/>
@@ -4856,39 +4815,39 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="56" t="n">
+      <c r="D2" s="46" t="n">
         <f aca="false">ROUND(2*D3*D4/(D3+D4),3)</f>
         <v>0.759</v>
       </c>
-      <c r="E2" s="56" t="n">
+      <c r="E2" s="46" t="n">
         <f aca="false">ROUND(2*E3*E4/(E3+E4),3)</f>
         <v>0.748</v>
       </c>
-      <c r="F2" s="56" t="n">
+      <c r="F2" s="46" t="n">
         <f aca="false">ROUND(2*F3*F4/(F3+F4),3)</f>
         <v>0.683</v>
       </c>
-      <c r="G2" s="56" t="n">
+      <c r="G2" s="46" t="n">
         <f aca="false">ROUND(2*G3*G4/(G3+G4),3)</f>
         <v>0.682</v>
       </c>
-      <c r="H2" s="56" t="n">
+      <c r="H2" s="46" t="n">
         <f aca="false">ROUND(2*H3*H4/(H3+H4),3)</f>
         <v>0.686</v>
       </c>
-      <c r="I2" s="56" t="n">
+      <c r="I2" s="46" t="n">
         <f aca="false">ROUND(2*I3*I4/(I3+I4),3)</f>
         <v>0.801</v>
       </c>
-      <c r="J2" s="56" t="n">
+      <c r="J2" s="46" t="n">
         <f aca="false">ROUND(2*J3*J4/(J3+J4),3)</f>
         <v>0.82</v>
       </c>
-      <c r="K2" s="56" t="n">
+      <c r="K2" s="46" t="n">
         <f aca="false">ROUND(2*K3*K4/(K3+K4),3)</f>
         <v>0.801</v>
       </c>
-      <c r="L2" s="57" t="n">
+      <c r="L2" s="47" t="n">
         <f aca="false">ROUND(2*L3*L4/(L3+L4),3)</f>
         <v>0.823</v>
       </c>
@@ -4920,7 +4879,7 @@
       <c r="I3" s="3" t="n">
         <v>0.782</v>
       </c>
-      <c r="J3" s="58" t="n">
+      <c r="J3" s="48" t="n">
         <v>0.807</v>
       </c>
       <c r="K3" s="3" t="n">
@@ -4965,7 +4924,7 @@
       <c r="K4" s="3" t="n">
         <v>0.818</v>
       </c>
-      <c r="L4" s="58" t="n">
+      <c r="L4" s="48" t="n">
         <v>0.84</v>
       </c>
       <c r="M4" s="14"/>
@@ -5018,39 +4977,39 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="56" t="n">
+      <c r="D6" s="46" t="n">
         <f aca="false">ROUND(2*D7*D8/(D7+D8),3)</f>
         <v>0.776</v>
       </c>
-      <c r="E6" s="56" t="n">
+      <c r="E6" s="46" t="n">
         <f aca="false">ROUND(2*E7*E8/(E7+E8),3)</f>
         <v>0.762</v>
       </c>
-      <c r="F6" s="56" t="n">
+      <c r="F6" s="46" t="n">
         <f aca="false">ROUND(2*F7*F8/(F7+F8),3)</f>
         <v>0.708</v>
       </c>
-      <c r="G6" s="56" t="n">
+      <c r="G6" s="46" t="n">
         <f aca="false">ROUND(2*G7*G8/(G7+G8),3)</f>
         <v>0.721</v>
       </c>
-      <c r="H6" s="56" t="n">
+      <c r="H6" s="46" t="n">
         <f aca="false">ROUND(2*H7*H8/(H7+H8),3)</f>
         <v>0.734</v>
       </c>
-      <c r="I6" s="56" t="n">
+      <c r="I6" s="46" t="n">
         <f aca="false">ROUND(2*I7*I8/(I7+I8),3)</f>
         <v>0.81</v>
       </c>
-      <c r="J6" s="56" t="n">
+      <c r="J6" s="46" t="n">
         <f aca="false">ROUND(2*J7*J8/(J7+J8),3)</f>
         <v>0.833</v>
       </c>
-      <c r="K6" s="56" t="n">
+      <c r="K6" s="46" t="n">
         <f aca="false">ROUND(2*K7*K8/(K7+K8),3)</f>
         <v>0.812</v>
       </c>
-      <c r="L6" s="57" t="n">
+      <c r="L6" s="47" t="n">
         <f aca="false">ROUND(2*L7*L8/(L7+L8),3)</f>
         <v>0.835</v>
       </c>
@@ -5083,7 +5042,7 @@
       <c r="I7" s="3" t="n">
         <v>0.788</v>
       </c>
-      <c r="J7" s="58" t="n">
+      <c r="J7" s="48" t="n">
         <v>0.815</v>
       </c>
       <c r="K7" s="3" t="n">
@@ -5129,7 +5088,7 @@
       <c r="K8" s="3" t="n">
         <v>0.833</v>
       </c>
-      <c r="L8" s="58" t="n">
+      <c r="L8" s="48" t="n">
         <v>0.858</v>
       </c>
       <c r="M8" s="14"/>
@@ -5145,39 +5104,39 @@
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="56" t="n">
+      <c r="D9" s="46" t="n">
         <f aca="false">ROUND(2*D10*D11/(D10+D11),3)</f>
         <v>0.761</v>
       </c>
-      <c r="E9" s="56" t="n">
+      <c r="E9" s="46" t="n">
         <f aca="false">ROUND(2*E10*E11/(E10+E11),3)</f>
         <v>0.734</v>
       </c>
-      <c r="F9" s="56" t="n">
+      <c r="F9" s="46" t="n">
         <f aca="false">ROUND(2*F10*F11/(F10+F11),3)</f>
         <v>0.63</v>
       </c>
-      <c r="G9" s="56" t="n">
+      <c r="G9" s="46" t="n">
         <f aca="false">ROUND(2*G10*G11/(G10+G11),3)</f>
         <v>0.82</v>
       </c>
-      <c r="H9" s="56" t="n">
+      <c r="H9" s="46" t="n">
         <f aca="false">ROUND(2*H10*H11/(H10+H11),3)</f>
         <v>0.845</v>
       </c>
-      <c r="I9" s="56" t="n">
+      <c r="I9" s="46" t="n">
         <f aca="false">ROUND(2*I10*I11/(I10+I11),3)</f>
         <v>0.888</v>
       </c>
-      <c r="J9" s="56" t="n">
+      <c r="J9" s="46" t="n">
         <f aca="false">ROUND(2*J10*J11/(J10+J11),3)</f>
         <v>0.89</v>
       </c>
-      <c r="K9" s="56" t="n">
+      <c r="K9" s="46" t="n">
         <f aca="false">ROUND(2*K10*K11/(K10+K11),3)</f>
         <v>0.888</v>
       </c>
-      <c r="L9" s="57" t="n">
+      <c r="L9" s="47" t="n">
         <f aca="false">ROUND(2*L10*L11/(L10+L11),3)</f>
         <v>0.891</v>
       </c>
@@ -5207,13 +5166,13 @@
       <c r="H10" s="3" t="n">
         <v>0.84</v>
       </c>
-      <c r="I10" s="58" t="n">
+      <c r="I10" s="48" t="n">
         <v>0.893</v>
       </c>
       <c r="J10" s="3" t="n">
         <v>0.89</v>
       </c>
-      <c r="K10" s="58" t="n">
+      <c r="K10" s="48" t="n">
         <v>0.893</v>
       </c>
       <c r="L10" s="3" t="n">
@@ -5250,13 +5209,13 @@
       <c r="I11" s="3" t="n">
         <v>0.883</v>
       </c>
-      <c r="J11" s="58" t="n">
+      <c r="J11" s="48" t="n">
         <v>0.89</v>
       </c>
       <c r="K11" s="3" t="n">
         <v>0.883</v>
       </c>
-      <c r="L11" s="58" t="n">
+      <c r="L11" s="48" t="n">
         <v>0.89</v>
       </c>
       <c r="M11" s="14"/>
@@ -5272,39 +5231,39 @@
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="56" t="n">
+      <c r="D12" s="46" t="n">
         <f aca="false">ROUND(2*D13*D14/(D13+D14),3)</f>
         <v>0.797</v>
       </c>
-      <c r="E12" s="57" t="n">
+      <c r="E12" s="47" t="n">
         <f aca="false">ROUND(2*E13*E14/(E13+E14),3)</f>
         <v>0.803</v>
       </c>
-      <c r="F12" s="56" t="n">
+      <c r="F12" s="46" t="n">
         <f aca="false">ROUND(2*F13*F14/(F13+F14),3)</f>
         <v>0.756</v>
       </c>
-      <c r="G12" s="56" t="n">
+      <c r="G12" s="46" t="n">
         <f aca="false">ROUND(2*G13*G14/(G13+G14),3)</f>
         <v>0.72</v>
       </c>
-      <c r="H12" s="56" t="n">
+      <c r="H12" s="46" t="n">
         <f aca="false">ROUND(2*H13*H14/(H13+H14),3)</f>
         <v>0.723</v>
       </c>
-      <c r="I12" s="56" t="n">
+      <c r="I12" s="46" t="n">
         <f aca="false">ROUND(2*I13*I14/(I13+I14),3)</f>
         <v>0.747</v>
       </c>
-      <c r="J12" s="56" t="n">
+      <c r="J12" s="46" t="n">
         <f aca="false">ROUND(2*J13*J14/(J13+J14),3)</f>
         <v>0.773</v>
       </c>
-      <c r="K12" s="56" t="n">
+      <c r="K12" s="46" t="n">
         <f aca="false">ROUND(2*K13*K14/(K13+K14),3)</f>
         <v>0.76</v>
       </c>
-      <c r="L12" s="56" t="n">
+      <c r="L12" s="46" t="n">
         <f aca="false">ROUND(2*L13*L14/(L13+L14),3)</f>
         <v>0.757</v>
       </c>
@@ -5321,7 +5280,7 @@
       <c r="D13" s="3" t="n">
         <v>0.799</v>
       </c>
-      <c r="E13" s="58" t="n">
+      <c r="E13" s="48" t="n">
         <v>0.805</v>
       </c>
       <c r="F13" s="3" t="n">
@@ -5360,7 +5319,7 @@
       <c r="D14" s="3" t="n">
         <v>0.795</v>
       </c>
-      <c r="E14" s="58" t="n">
+      <c r="E14" s="48" t="n">
         <v>0.801</v>
       </c>
       <c r="F14" s="3" t="n">
@@ -5434,39 +5393,39 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="57" t="n">
+      <c r="D16" s="47" t="n">
         <f aca="false">ROUND(2*D17*D18/(D17+D18),3)</f>
         <v>0.817</v>
       </c>
-      <c r="E16" s="56" t="n">
+      <c r="E16" s="46" t="n">
         <f aca="false">ROUND(2*E17*E18/(E17+E18),3)</f>
         <v>0.813</v>
       </c>
-      <c r="F16" s="56" t="n">
+      <c r="F16" s="46" t="n">
         <f aca="false">ROUND(2*F17*F18/(F17+F18),3)</f>
         <v>0.763</v>
       </c>
-      <c r="G16" s="56" t="n">
+      <c r="G16" s="46" t="n">
         <f aca="false">ROUND(2*G17*G18/(G17+G18),3)</f>
         <v>0.759</v>
       </c>
-      <c r="H16" s="56" t="n">
+      <c r="H16" s="46" t="n">
         <f aca="false">ROUND(2*H17*H18/(H17+H18),3)</f>
         <v>0.763</v>
       </c>
-      <c r="I16" s="56" t="n">
+      <c r="I16" s="46" t="n">
         <f aca="false">ROUND(2*I17*I18/(I17+I18),3)</f>
         <v>0.763</v>
       </c>
-      <c r="J16" s="56" t="n">
+      <c r="J16" s="46" t="n">
         <f aca="false">ROUND(2*J17*J18/(J17+J18),3)</f>
         <v>0.794</v>
       </c>
-      <c r="K16" s="56" t="n">
+      <c r="K16" s="46" t="n">
         <f aca="false">ROUND(2*K17*K18/(K17+K18),3)</f>
         <v>0.772</v>
       </c>
-      <c r="L16" s="56" t="n">
+      <c r="L16" s="46" t="n">
         <f aca="false">ROUND(2*L17*L18/(L17+L18),3)</f>
         <v>0.783</v>
       </c>
@@ -5484,7 +5443,7 @@
       <c r="D17" s="3" t="n">
         <v>0.82</v>
       </c>
-      <c r="E17" s="58" t="n">
+      <c r="E17" s="48" t="n">
         <v>0.821</v>
       </c>
       <c r="F17" s="3" t="n">
@@ -5521,7 +5480,7 @@
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="58" t="n">
+      <c r="D18" s="48" t="n">
         <v>0.814</v>
       </c>
       <c r="E18" s="3" t="n">
@@ -5561,39 +5520,39 @@
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="56" t="n">
+      <c r="D19" s="46" t="n">
         <f aca="false">ROUND(2*D20*D21/(D20+D21),3)</f>
         <v>0.785</v>
       </c>
-      <c r="E19" s="56" t="n">
+      <c r="E19" s="46" t="n">
         <f aca="false">ROUND(2*E20*E21/(E20+E21),3)</f>
         <v>0.755</v>
       </c>
-      <c r="F19" s="56" t="n">
+      <c r="F19" s="46" t="n">
         <f aca="false">ROUND(2*F20*F21/(F20+F21),3)</f>
         <v>0.676</v>
       </c>
-      <c r="G19" s="56" t="n">
+      <c r="G19" s="46" t="n">
         <f aca="false">ROUND(2*G20*G21/(G20+G21),3)</f>
         <v>0.837</v>
       </c>
-      <c r="H19" s="56" t="n">
+      <c r="H19" s="46" t="n">
         <f aca="false">ROUND(2*H20*H21/(H20+H21),3)</f>
         <v>0.857</v>
       </c>
-      <c r="I19" s="56" t="n">
+      <c r="I19" s="46" t="n">
         <f aca="false">ROUND(2*I20*I21/(I20+I21),3)</f>
         <v>0.89</v>
       </c>
-      <c r="J19" s="56" t="n">
+      <c r="J19" s="46" t="n">
         <f aca="false">ROUND(2*J20*J21/(J20+J21),3)</f>
         <v>0.882</v>
       </c>
-      <c r="K19" s="57" t="n">
+      <c r="K19" s="47" t="n">
         <f aca="false">ROUND(2*K20*K21/(K20+K21),3)</f>
         <v>0.892</v>
       </c>
-      <c r="L19" s="56" t="n">
+      <c r="L19" s="46" t="n">
         <f aca="false">ROUND(2*L20*L21/(L20+L21),3)</f>
         <v>0.884</v>
       </c>
@@ -5623,13 +5582,13 @@
       <c r="H20" s="3" t="n">
         <v>0.848</v>
       </c>
-      <c r="I20" s="58" t="n">
+      <c r="I20" s="48" t="n">
         <v>0.888</v>
       </c>
       <c r="J20" s="3" t="n">
         <v>0.878</v>
       </c>
-      <c r="K20" s="58" t="n">
+      <c r="K20" s="48" t="n">
         <v>0.888</v>
       </c>
       <c r="L20" s="3" t="n">
@@ -5669,7 +5628,7 @@
       <c r="J21" s="3" t="n">
         <v>0.887</v>
       </c>
-      <c r="K21" s="58" t="n">
+      <c r="K21" s="48" t="n">
         <v>0.896</v>
       </c>
       <c r="L21" s="3" t="n">
@@ -5688,39 +5647,36 @@
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="56" t="n">
+      <c r="D22" s="46" t="n">
         <f aca="false">ROUND(2*D23*D24/(D23+D24),3)</f>
         <v>0.707</v>
       </c>
-      <c r="E22" s="57" t="n">
+      <c r="E22" s="47" t="n">
         <f aca="false">ROUND(2*E23*E24/(E23+E24),3)</f>
         <v>0.736</v>
       </c>
-      <c r="F22" s="56" t="e">
-        <f aca="false">ROUND(2*F23*F24/(F23+F24),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="56" t="n">
+      <c r="F22" s="49"/>
+      <c r="G22" s="46" t="n">
         <f aca="false">ROUND(2*G23*G24/(G23+G24),3)</f>
         <v>0.632</v>
       </c>
-      <c r="H22" s="56" t="n">
+      <c r="H22" s="46" t="n">
         <f aca="false">ROUND(2*H23*H24/(H23+H24),3)</f>
         <v>0.633</v>
       </c>
-      <c r="I22" s="56" t="n">
+      <c r="I22" s="46" t="n">
         <f aca="false">ROUND(2*I23*I24/(I23+I24),3)</f>
         <v>0.584</v>
       </c>
-      <c r="J22" s="56" t="n">
+      <c r="J22" s="46" t="n">
         <f aca="false">ROUND(2*J23*J24/(J23+J24),3)</f>
         <v>0.602</v>
       </c>
-      <c r="K22" s="56" t="n">
+      <c r="K22" s="46" t="n">
         <f aca="false">ROUND(2*K23*K24/(K23+K24),3)</f>
         <v>0.607</v>
       </c>
-      <c r="L22" s="56" t="n">
+      <c r="L22" s="46" t="n">
         <f aca="false">ROUND(2*L23*L24/(L23+L24),3)</f>
         <v>0.579</v>
       </c>
@@ -5737,10 +5693,10 @@
       <c r="D23" s="3" t="n">
         <v>0.738</v>
       </c>
-      <c r="E23" s="58" t="n">
+      <c r="E23" s="48" t="n">
         <v>0.761</v>
       </c>
-      <c r="F23" s="44"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="3" t="n">
         <v>0.65</v>
       </c>
@@ -5750,13 +5706,13 @@
       <c r="I23" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="J23" s="45" t="n">
+      <c r="J23" s="3" t="n">
         <v>0.614</v>
       </c>
-      <c r="K23" s="45" t="n">
+      <c r="K23" s="3" t="n">
         <v>0.634</v>
       </c>
-      <c r="L23" s="45" t="n">
+      <c r="L23" s="3" t="n">
         <v>0.589</v>
       </c>
       <c r="M23" s="14"/>
@@ -5774,10 +5730,10 @@
       <c r="D24" s="3" t="n">
         <v>0.679</v>
       </c>
-      <c r="E24" s="58" t="n">
+      <c r="E24" s="48" t="n">
         <v>0.713</v>
       </c>
-      <c r="F24" s="44"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="3" t="n">
         <v>0.615</v>
       </c>
@@ -5787,13 +5743,13 @@
       <c r="I24" s="3" t="n">
         <v>0.569</v>
       </c>
-      <c r="J24" s="45" t="n">
+      <c r="J24" s="3" t="n">
         <v>0.59</v>
       </c>
-      <c r="K24" s="45" t="n">
+      <c r="K24" s="3" t="n">
         <v>0.583</v>
       </c>
-      <c r="L24" s="45" t="n">
+      <c r="L24" s="3" t="n">
         <v>0.57</v>
       </c>
       <c r="M24" s="14"/>
@@ -5810,7 +5766,7 @@
       <c r="E25" s="3" t="n">
         <v>212.5</v>
       </c>
-      <c r="F25" s="44"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="3" t="n">
         <v>12000.2</v>
       </c>
@@ -5820,13 +5776,13 @@
       <c r="I25" s="3" t="n">
         <v>1482.4</v>
       </c>
-      <c r="J25" s="45" t="n">
+      <c r="J25" s="3" t="n">
         <v>28858.6</v>
       </c>
-      <c r="K25" s="45" t="n">
+      <c r="K25" s="3" t="n">
         <v>28777.5</v>
       </c>
-      <c r="L25" s="45" t="n">
+      <c r="L25" s="3" t="n">
         <v>28604.9</v>
       </c>
       <c r="M25" s="14"/>
@@ -5844,39 +5800,36 @@
       <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="57" t="n">
+      <c r="D26" s="47" t="n">
         <f aca="false">ROUND(2*D27*D28/(D27+D28),3)</f>
         <v>0.8</v>
       </c>
-      <c r="E26" s="56" t="n">
+      <c r="E26" s="46" t="n">
         <f aca="false">ROUND(2*E27*E28/(E27+E28),3)</f>
         <v>0.79</v>
       </c>
-      <c r="F26" s="56" t="e">
-        <f aca="false">ROUND(2*F27*F28/(F27+F28),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="56" t="n">
+      <c r="F26" s="49"/>
+      <c r="G26" s="46" t="n">
         <f aca="false">ROUND(2*G27*G28/(G27+G28),3)</f>
         <v>0.744</v>
       </c>
-      <c r="H26" s="56" t="n">
+      <c r="H26" s="46" t="n">
         <f aca="false">ROUND(2*H27*H28/(H27+H28),3)</f>
         <v>0.75</v>
       </c>
-      <c r="I26" s="56" t="n">
+      <c r="I26" s="46" t="n">
         <f aca="false">ROUND(2*I27*I28/(I27+I28),3)</f>
         <v>0.769</v>
       </c>
-      <c r="J26" s="56" t="n">
+      <c r="J26" s="46" t="n">
         <f aca="false">ROUND(2*J27*J28/(J27+J28),3)</f>
         <v>0.779</v>
       </c>
-      <c r="K26" s="56" t="n">
+      <c r="K26" s="46" t="n">
         <f aca="false">ROUND(2*K27*K28/(K27+K28),3)</f>
         <v>0.784</v>
       </c>
-      <c r="L26" s="56" t="n">
+      <c r="L26" s="46" t="n">
         <f aca="false">ROUND(2*L27*L28/(L27+L28),3)</f>
         <v>0.769</v>
       </c>
@@ -5891,13 +5844,13 @@
       <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="58" t="n">
+      <c r="D27" s="48" t="n">
         <v>0.811</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>0.802</v>
       </c>
-      <c r="F27" s="44"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="3" t="n">
         <v>0.747</v>
       </c>
@@ -5907,13 +5860,13 @@
       <c r="I27" s="3" t="n">
         <v>0.762</v>
       </c>
-      <c r="J27" s="45" t="n">
+      <c r="J27" s="3" t="n">
         <v>0.782</v>
       </c>
-      <c r="K27" s="45" t="n">
+      <c r="K27" s="3" t="n">
         <v>0.778</v>
       </c>
-      <c r="L27" s="45" t="n">
+      <c r="L27" s="3" t="n">
         <v>0.769</v>
       </c>
       <c r="M27" s="14"/>
@@ -5935,7 +5888,7 @@
       <c r="E28" s="3" t="n">
         <v>0.778</v>
       </c>
-      <c r="F28" s="44"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="3" t="n">
         <v>0.741</v>
       </c>
@@ -5945,13 +5898,13 @@
       <c r="I28" s="3" t="n">
         <v>0.777</v>
       </c>
-      <c r="J28" s="45" t="n">
+      <c r="J28" s="3" t="n">
         <v>0.777</v>
       </c>
-      <c r="K28" s="59" t="n">
+      <c r="K28" s="48" t="n">
         <v>0.791</v>
       </c>
-      <c r="L28" s="45" t="n">
+      <c r="L28" s="3" t="n">
         <v>0.77</v>
       </c>
       <c r="M28" s="14"/>
@@ -5967,39 +5920,36 @@
       <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="56" t="n">
+      <c r="D29" s="46" t="n">
         <f aca="false">ROUND(2*D30*D31/(D30+D31),3)</f>
         <v>0.799</v>
       </c>
-      <c r="E29" s="56" t="n">
+      <c r="E29" s="46" t="n">
         <f aca="false">ROUND(2*E30*E31/(E30+E31),3)</f>
         <v>0.802</v>
       </c>
-      <c r="F29" s="56" t="e">
-        <f aca="false">ROUND(2*F30*F31/(F30+F31),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="56" t="n">
+      <c r="F29" s="49"/>
+      <c r="G29" s="46" t="n">
         <f aca="false">ROUND(2*G30*G31/(G30+G31),3)</f>
         <v>0.803</v>
       </c>
-      <c r="H29" s="56" t="n">
+      <c r="H29" s="46" t="n">
         <f aca="false">ROUND(2*H30*H31/(H30+H31),3)</f>
         <v>0.827</v>
       </c>
-      <c r="I29" s="56" t="n">
+      <c r="I29" s="46" t="n">
         <f aca="false">ROUND(2*I30*I31/(I30+I31),3)</f>
         <v>0.848</v>
       </c>
-      <c r="J29" s="56" t="n">
+      <c r="J29" s="46" t="n">
         <f aca="false">ROUND(2*J30*J31/(J30+J31),3)</f>
         <v>0.846</v>
       </c>
-      <c r="K29" s="57" t="n">
+      <c r="K29" s="47" t="n">
         <f aca="false">ROUND(2*K30*K31/(K30+K31),3)</f>
         <v>0.862</v>
       </c>
-      <c r="L29" s="56" t="n">
+      <c r="L29" s="46" t="n">
         <f aca="false">ROUND(2*L30*L31/(L30+L31),3)</f>
         <v>0.84</v>
       </c>
@@ -6020,7 +5970,7 @@
       <c r="E30" s="3" t="n">
         <v>0.797</v>
       </c>
-      <c r="F30" s="44"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="3" t="n">
         <v>0.812</v>
       </c>
@@ -6030,13 +5980,13 @@
       <c r="I30" s="3" t="n">
         <v>0.858</v>
       </c>
-      <c r="J30" s="45" t="n">
+      <c r="J30" s="3" t="n">
         <v>0.857</v>
       </c>
-      <c r="K30" s="59" t="n">
+      <c r="K30" s="48" t="n">
         <v>0.869</v>
       </c>
-      <c r="L30" s="45" t="n">
+      <c r="L30" s="3" t="n">
         <v>0.85</v>
       </c>
       <c r="M30" s="14"/>
@@ -6058,7 +6008,7 @@
       <c r="E31" s="3" t="n">
         <v>0.807</v>
       </c>
-      <c r="F31" s="44"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="3" t="n">
         <v>0.794</v>
       </c>
@@ -6068,13 +6018,13 @@
       <c r="I31" s="3" t="n">
         <v>0.839</v>
       </c>
-      <c r="J31" s="45" t="n">
+      <c r="J31" s="3" t="n">
         <v>0.836</v>
       </c>
-      <c r="K31" s="59" t="n">
+      <c r="K31" s="48" t="n">
         <v>0.855</v>
       </c>
-      <c r="L31" s="45" t="n">
+      <c r="L31" s="3" t="n">
         <v>0.831</v>
       </c>
       <c r="M31" s="14"/>
@@ -6090,39 +6040,39 @@
       <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="56" t="n">
+      <c r="D32" s="46" t="n">
         <f aca="false">ROUND(2*D33*D34/(D33+D34),3)</f>
         <v>0.756</v>
       </c>
-      <c r="E32" s="56" t="n">
+      <c r="E32" s="46" t="n">
         <f aca="false">ROUND(2*E33*E34/(E33+E34),3)</f>
         <v>0.738</v>
       </c>
-      <c r="F32" s="56" t="e">
+      <c r="F32" s="46" t="n">
         <f aca="false">ROUND(2*F33*F34/(F33+F34),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G32" s="56" t="n">
+        <v>0.647</v>
+      </c>
+      <c r="G32" s="46" t="n">
         <f aca="false">ROUND(2*G33*G34/(G33+G34),3)</f>
         <v>0.597</v>
       </c>
-      <c r="H32" s="56" t="n">
+      <c r="H32" s="46" t="n">
         <f aca="false">ROUND(2*H33*H34/(H33+H34),3)</f>
         <v>0.606</v>
       </c>
-      <c r="I32" s="56" t="n">
+      <c r="I32" s="46" t="n">
         <f aca="false">ROUND(2*I33*I34/(I33+I34),3)</f>
         <v>0.752</v>
       </c>
-      <c r="J32" s="57" t="n">
+      <c r="J32" s="47" t="n">
         <f aca="false">ROUND(2*J33*J34/(J33+J34),3)</f>
         <v>0.773</v>
       </c>
-      <c r="K32" s="56" t="n">
+      <c r="K32" s="46" t="n">
         <f aca="false">ROUND(2*K33*K34/(K33+K34),3)</f>
         <v>0.756</v>
       </c>
-      <c r="L32" s="56" t="n">
+      <c r="L32" s="46" t="n">
         <f aca="false">ROUND(2*L33*L34/(L33+L34),3)</f>
         <v>0.771</v>
       </c>
@@ -6134,13 +6084,15 @@
       <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="58" t="n">
+      <c r="D33" s="48" t="n">
         <v>0.772</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>0.75</v>
       </c>
-      <c r="F33" s="44"/>
+      <c r="F33" s="45" t="n">
+        <v>0.657</v>
+      </c>
       <c r="G33" s="3" t="n">
         <v>0.58</v>
       </c>
@@ -6173,7 +6125,9 @@
       <c r="E34" s="3" t="n">
         <v>0.726</v>
       </c>
-      <c r="F34" s="44"/>
+      <c r="F34" s="45" t="n">
+        <v>0.638</v>
+      </c>
       <c r="G34" s="3" t="n">
         <v>0.615</v>
       </c>
@@ -6183,7 +6137,7 @@
       <c r="I34" s="3" t="n">
         <v>0.779</v>
       </c>
-      <c r="J34" s="58" t="n">
+      <c r="J34" s="48" t="n">
         <v>0.795</v>
       </c>
       <c r="K34" s="3" t="n">
@@ -6204,7 +6158,9 @@
       <c r="E35" s="3" t="n">
         <v>259.1</v>
       </c>
-      <c r="F35" s="44"/>
+      <c r="F35" s="45" t="n">
+        <v>86705.3</v>
+      </c>
       <c r="G35" s="3" t="n">
         <v>8483.4</v>
       </c>
@@ -6234,39 +6190,39 @@
       <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="56" t="n">
+      <c r="D36" s="46" t="n">
         <f aca="false">ROUND(2*D37*D38/(D37+D38),3)</f>
         <v>0.772</v>
       </c>
-      <c r="E36" s="56" t="n">
+      <c r="E36" s="46" t="n">
         <f aca="false">ROUND(2*E37*E38/(E37+E38),3)</f>
         <v>0.753</v>
       </c>
-      <c r="F36" s="56" t="e">
+      <c r="F36" s="50" t="n">
         <f aca="false">ROUND(2*F37*F38/(F37+F38),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="56" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="G36" s="46" t="n">
         <f aca="false">ROUND(2*G37*G38/(G37+G38),3)</f>
         <v>0.76</v>
       </c>
-      <c r="H36" s="56" t="n">
+      <c r="H36" s="46" t="n">
         <f aca="false">ROUND(2*H37*H38/(H37+H38),3)</f>
         <v>0.771</v>
       </c>
-      <c r="I36" s="56" t="n">
+      <c r="I36" s="46" t="n">
         <f aca="false">ROUND(2*I37*I38/(I37+I38),3)</f>
         <v>0.826</v>
       </c>
-      <c r="J36" s="57" t="n">
+      <c r="J36" s="47" t="n">
         <f aca="false">ROUND(2*J37*J38/(J37+J38),3)</f>
         <v>0.846</v>
       </c>
-      <c r="K36" s="56" t="n">
+      <c r="K36" s="46" t="n">
         <f aca="false">ROUND(2*K37*K38/(K37+K38),3)</f>
         <v>0.828</v>
       </c>
-      <c r="L36" s="56" t="n">
+      <c r="L36" s="46" t="n">
         <f aca="false">ROUND(2*L37*L38/(L37+L38),3)</f>
         <v>0.845</v>
       </c>
@@ -6285,7 +6241,9 @@
       <c r="E37" s="3" t="n">
         <v>0.763</v>
       </c>
-      <c r="F37" s="44"/>
+      <c r="F37" s="45" t="n">
+        <v>0.68</v>
+      </c>
       <c r="G37" s="3" t="n">
         <v>0.75</v>
       </c>
@@ -6295,7 +6253,7 @@
       <c r="I37" s="3" t="n">
         <v>0.806</v>
       </c>
-      <c r="J37" s="58" t="n">
+      <c r="J37" s="48" t="n">
         <v>0.831</v>
       </c>
       <c r="K37" s="3" t="n">
@@ -6319,7 +6277,9 @@
       <c r="E38" s="3" t="n">
         <v>0.743</v>
       </c>
-      <c r="F38" s="44"/>
+      <c r="F38" s="45" t="n">
+        <v>0.65</v>
+      </c>
       <c r="G38" s="3" t="n">
         <v>0.77</v>
       </c>
@@ -6335,7 +6295,7 @@
       <c r="K38" s="3" t="n">
         <v>0.846</v>
       </c>
-      <c r="L38" s="58" t="n">
+      <c r="L38" s="48" t="n">
         <v>0.863</v>
       </c>
     </row>
@@ -6408,8 +6368,8 @@
   </sheetPr>
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6427,15 +6387,15 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -6473,29 +6433,31 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="61" t="n">
+      <c r="B4" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="n">
+      <c r="C4" s="52" t="n">
         <v>0.0504374219701802</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63" t="n">
+      <c r="D4" s="53" t="n">
+        <v>4.03621174251569E-040</v>
+      </c>
+      <c r="E4" s="53" t="n">
         <v>2.15693119619744E-032</v>
       </c>
-      <c r="F4" s="63" t="n">
+      <c r="F4" s="53" t="n">
         <v>1.14346370107601E-028</v>
       </c>
-      <c r="G4" s="63" t="n">
+      <c r="G4" s="53" t="n">
         <v>3.73199742961688E-006</v>
       </c>
-      <c r="H4" s="63" t="n">
+      <c r="H4" s="53" t="n">
         <v>7.6195945023728E-012</v>
       </c>
-      <c r="I4" s="63" t="n">
+      <c r="I4" s="53" t="n">
         <v>8.74126611158293E-006</v>
       </c>
-      <c r="J4" s="63" t="n">
+      <c r="J4" s="53" t="n">
         <v>7.34597418180524E-012</v>
       </c>
     </row>
@@ -6503,29 +6465,31 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="61" t="n">
+      <c r="B5" s="52" t="n">
         <v>0.0504374219701802</v>
       </c>
-      <c r="C5" s="61" t="n">
+      <c r="C5" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63" t="n">
+      <c r="D5" s="53" t="n">
+        <v>1.87427687363831E-029</v>
+      </c>
+      <c r="E5" s="53" t="n">
         <v>2.06540484386954E-025</v>
       </c>
-      <c r="F5" s="63" t="n">
+      <c r="F5" s="53" t="n">
         <v>3.86093209646504E-022</v>
       </c>
-      <c r="G5" s="63" t="n">
+      <c r="G5" s="53" t="n">
         <v>1.53288419089158E-010</v>
       </c>
-      <c r="H5" s="63" t="n">
+      <c r="H5" s="53" t="n">
         <v>6.20175996564841E-018</v>
       </c>
-      <c r="I5" s="63" t="n">
+      <c r="I5" s="53" t="n">
         <v>5.90018652347681E-010</v>
       </c>
-      <c r="J5" s="63" t="n">
+      <c r="J5" s="53" t="n">
         <v>5.08542553727978E-018</v>
       </c>
     </row>
@@ -6533,45 +6497,63 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="61" t="n">
+      <c r="B6" s="53" t="n">
+        <v>4.03621174251569E-040</v>
+      </c>
+      <c r="C6" s="53" t="n">
+        <v>1.87427687363831E-029</v>
+      </c>
+      <c r="D6" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
+      <c r="E6" s="52" t="n">
+        <v>0.029068864497185</v>
+      </c>
+      <c r="F6" s="52" t="n">
+        <v>0.154207912234445</v>
+      </c>
+      <c r="G6" s="53" t="n">
+        <v>3.24029986353632E-063</v>
+      </c>
+      <c r="H6" s="53" t="n">
+        <v>2.10418644095109E-081</v>
+      </c>
+      <c r="I6" s="53" t="n">
+        <v>1.86433463547439E-060</v>
+      </c>
+      <c r="J6" s="53" t="n">
+        <v>1.93272738657328E-082</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="63" t="n">
+      <c r="B7" s="53" t="n">
         <v>2.15693119619744E-032</v>
       </c>
-      <c r="C7" s="63" t="n">
+      <c r="C7" s="53" t="n">
         <v>2.06540484386954E-025</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="61" t="n">
+      <c r="D7" s="52" t="n">
+        <v>0.029068864497185</v>
+      </c>
+      <c r="E7" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="61" t="n">
+      <c r="F7" s="52" t="n">
         <v>0.533362718697031</v>
       </c>
-      <c r="G7" s="63" t="n">
+      <c r="G7" s="53" t="n">
         <v>4.88010674418018E-049</v>
       </c>
-      <c r="H7" s="63" t="n">
+      <c r="H7" s="53" t="n">
         <v>3.84237189509186E-060</v>
       </c>
-      <c r="I7" s="63" t="n">
+      <c r="I7" s="53" t="n">
         <v>1.13321619289739E-047</v>
       </c>
-      <c r="J7" s="63" t="n">
+      <c r="J7" s="53" t="n">
         <v>1.9265289826061E-060</v>
       </c>
     </row>
@@ -6579,29 +6561,31 @@
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="63" t="n">
+      <c r="B8" s="53" t="n">
         <v>1.14346370107601E-028</v>
       </c>
-      <c r="C8" s="63" t="n">
+      <c r="C8" s="53" t="n">
         <v>3.86093209646504E-022</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="61" t="n">
+      <c r="D8" s="52" t="n">
+        <v>0.154207912234445</v>
+      </c>
+      <c r="E8" s="52" t="n">
         <v>0.533362718697031</v>
       </c>
-      <c r="F8" s="61" t="n">
+      <c r="F8" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="63" t="n">
+      <c r="G8" s="53" t="n">
         <v>1.24002979588012E-044</v>
       </c>
-      <c r="H8" s="63" t="n">
+      <c r="H8" s="53" t="n">
         <v>3.17240337783778E-055</v>
       </c>
-      <c r="I8" s="63" t="n">
+      <c r="I8" s="53" t="n">
         <v>2.25965683942311E-043</v>
       </c>
-      <c r="J8" s="63" t="n">
+      <c r="J8" s="53" t="n">
         <v>1.74180322258743E-055</v>
       </c>
     </row>
@@ -6609,29 +6593,31 @@
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="63" t="n">
+      <c r="B9" s="53" t="n">
         <v>3.73199742961688E-006</v>
       </c>
-      <c r="C9" s="63" t="n">
+      <c r="C9" s="53" t="n">
         <v>1.53288419089158E-010</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="63" t="n">
+      <c r="D9" s="53" t="n">
+        <v>3.24029986353632E-063</v>
+      </c>
+      <c r="E9" s="53" t="n">
         <v>4.88010674418018E-049</v>
       </c>
-      <c r="F9" s="63" t="n">
+      <c r="F9" s="53" t="n">
         <v>1.24002979588012E-044</v>
       </c>
-      <c r="G9" s="61" t="n">
+      <c r="G9" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="61" t="n">
+      <c r="H9" s="52" t="n">
         <v>0.0469885584080821</v>
       </c>
-      <c r="I9" s="61" t="n">
+      <c r="I9" s="52" t="n">
         <v>0.930949590132206</v>
       </c>
-      <c r="J9" s="61" t="n">
+      <c r="J9" s="52" t="n">
         <v>0.0522339283086912</v>
       </c>
     </row>
@@ -6639,29 +6625,31 @@
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="63" t="n">
+      <c r="B10" s="53" t="n">
         <v>7.6195945023728E-012</v>
       </c>
-      <c r="C10" s="63" t="n">
+      <c r="C10" s="53" t="n">
         <v>6.20175996564841E-018</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63" t="n">
+      <c r="D10" s="53" t="n">
+        <v>2.10418644095109E-081</v>
+      </c>
+      <c r="E10" s="53" t="n">
         <v>3.84237189509186E-060</v>
       </c>
-      <c r="F10" s="63" t="n">
+      <c r="F10" s="53" t="n">
         <v>3.17240337783778E-055</v>
       </c>
-      <c r="G10" s="61" t="n">
+      <c r="G10" s="52" t="n">
         <v>0.0469885584080821</v>
       </c>
-      <c r="H10" s="61" t="n">
+      <c r="H10" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="61" t="n">
+      <c r="I10" s="52" t="n">
         <v>0.0414958759510203</v>
       </c>
-      <c r="J10" s="61" t="n">
+      <c r="J10" s="52" t="n">
         <v>0.947247110452291</v>
       </c>
     </row>
@@ -6669,29 +6657,31 @@
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="63" t="n">
+      <c r="B11" s="53" t="n">
         <v>8.74126611158293E-006</v>
       </c>
-      <c r="C11" s="63" t="n">
+      <c r="C11" s="53" t="n">
         <v>5.90018652347681E-010</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63" t="n">
+      <c r="D11" s="53" t="n">
+        <v>1.86433463547439E-060</v>
+      </c>
+      <c r="E11" s="53" t="n">
         <v>1.13321619289739E-047</v>
       </c>
-      <c r="F11" s="63" t="n">
+      <c r="F11" s="53" t="n">
         <v>2.25965683942311E-043</v>
       </c>
-      <c r="G11" s="61" t="n">
+      <c r="G11" s="52" t="n">
         <v>0.930949590132206</v>
       </c>
-      <c r="H11" s="61" t="n">
+      <c r="H11" s="52" t="n">
         <v>0.0414958759510203</v>
       </c>
-      <c r="I11" s="61" t="n">
+      <c r="I11" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="61" t="n">
+      <c r="J11" s="52" t="n">
         <v>0.0461163943063906</v>
       </c>
     </row>
@@ -6699,29 +6689,31 @@
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="63" t="n">
+      <c r="B12" s="53" t="n">
         <v>7.34597418180524E-012</v>
       </c>
-      <c r="C12" s="63" t="n">
+      <c r="C12" s="53" t="n">
         <v>5.08542553727978E-018</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="63" t="n">
+      <c r="D12" s="53" t="n">
+        <v>1.93272738657328E-082</v>
+      </c>
+      <c r="E12" s="53" t="n">
         <v>1.9265289826061E-060</v>
       </c>
-      <c r="F12" s="63" t="n">
+      <c r="F12" s="53" t="n">
         <v>1.74180322258743E-055</v>
       </c>
-      <c r="G12" s="61" t="n">
+      <c r="G12" s="52" t="n">
         <v>0.0522339283086912</v>
       </c>
-      <c r="H12" s="61" t="n">
+      <c r="H12" s="52" t="n">
         <v>0.947247110452291</v>
       </c>
-      <c r="I12" s="61" t="n">
+      <c r="I12" s="52" t="n">
         <v>0.0461163943063906</v>
       </c>
-      <c r="J12" s="61" t="n">
+      <c r="J12" s="52" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6773,29 +6765,31 @@
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="61" t="n">
+      <c r="B15" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="61" t="n">
+      <c r="C15" s="52" t="n">
         <v>0.0464204936614076</v>
       </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="61" t="n">
+      <c r="D15" s="53" t="n">
+        <v>1.11886995766341E-029</v>
+      </c>
+      <c r="E15" s="52" t="n">
         <v>0.430766044004024</v>
       </c>
-      <c r="F15" s="61" t="n">
+      <c r="F15" s="52" t="n">
         <v>0.0337628569558176</v>
       </c>
-      <c r="G15" s="63" t="n">
+      <c r="G15" s="53" t="n">
         <v>1.40569225114268E-022</v>
       </c>
-      <c r="H15" s="63" t="n">
+      <c r="H15" s="53" t="n">
         <v>2.44727963532734E-033</v>
       </c>
-      <c r="I15" s="63" t="n">
+      <c r="I15" s="53" t="n">
         <v>2.30741482669337E-021</v>
       </c>
-      <c r="J15" s="63" t="n">
+      <c r="J15" s="53" t="n">
         <v>7.68464116569817E-035</v>
       </c>
     </row>
@@ -6803,29 +6797,31 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="61" t="n">
+      <c r="B16" s="52" t="n">
         <v>0.0464204936614076</v>
       </c>
-      <c r="C16" s="61" t="n">
+      <c r="C16" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="63" t="n">
+      <c r="D16" s="53" t="n">
+        <v>6.69869287499587E-021</v>
+      </c>
+      <c r="E16" s="53" t="n">
         <v>0.00807972941599414</v>
       </c>
-      <c r="F16" s="63" t="n">
+      <c r="F16" s="53" t="n">
         <v>5.89302677569622E-005</v>
       </c>
-      <c r="G16" s="63" t="n">
+      <c r="G16" s="53" t="n">
         <v>1.71965848370678E-031</v>
       </c>
-      <c r="H16" s="63" t="n">
+      <c r="H16" s="53" t="n">
         <v>4.25216928403771E-044</v>
       </c>
-      <c r="I16" s="63" t="n">
+      <c r="I16" s="53" t="n">
         <v>5.64415485286877E-030</v>
       </c>
-      <c r="J16" s="63" t="n">
+      <c r="J16" s="53" t="n">
         <v>8.08808335907419E-046</v>
       </c>
     </row>
@@ -6833,45 +6829,63 @@
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="61" t="n">
+      <c r="B17" s="53" t="n">
+        <v>1.11886995766341E-029</v>
+      </c>
+      <c r="C17" s="53" t="n">
+        <v>6.69869287499587E-021</v>
+      </c>
+      <c r="D17" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="E17" s="53" t="n">
+        <v>5.04952182463349E-030</v>
+      </c>
+      <c r="F17" s="53" t="n">
+        <v>6.9156148927919E-038</v>
+      </c>
+      <c r="G17" s="53" t="n">
+        <v>5.45548936585914E-093</v>
+      </c>
+      <c r="H17" s="53" t="n">
+        <v>1.81322635172938E-114</v>
+      </c>
+      <c r="I17" s="53" t="n">
+        <v>8.03709397994766E-090</v>
+      </c>
+      <c r="J17" s="53" t="n">
+        <v>3.18649308951078E-117</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="61" t="n">
+      <c r="B18" s="52" t="n">
         <v>0.430766044004024</v>
       </c>
-      <c r="C18" s="63" t="n">
+      <c r="C18" s="53" t="n">
         <v>0.00807972941599414</v>
       </c>
-      <c r="D18" s="62"/>
-      <c r="E18" s="61" t="n">
+      <c r="D18" s="53" t="n">
+        <v>5.04952182463349E-030</v>
+      </c>
+      <c r="E18" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="61" t="n">
+      <c r="F18" s="52" t="n">
         <v>0.216477102752999</v>
       </c>
-      <c r="G18" s="63" t="n">
+      <c r="G18" s="53" t="n">
         <v>1.41295460619338E-016</v>
       </c>
-      <c r="H18" s="63" t="n">
+      <c r="H18" s="53" t="n">
         <v>1.18149166843919E-024</v>
       </c>
-      <c r="I18" s="63" t="n">
+      <c r="I18" s="53" t="n">
         <v>1.04626200407502E-015</v>
       </c>
-      <c r="J18" s="63" t="n">
+      <c r="J18" s="53" t="n">
         <v>8.79815661908534E-026</v>
       </c>
     </row>
@@ -6879,29 +6893,31 @@
       <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="61" t="n">
+      <c r="B19" s="52" t="n">
         <v>0.0337628569558176</v>
       </c>
-      <c r="C19" s="63" t="n">
+      <c r="C19" s="53" t="n">
         <v>5.89302677569622E-005</v>
       </c>
-      <c r="D19" s="62"/>
-      <c r="E19" s="61" t="n">
+      <c r="D19" s="53" t="n">
+        <v>6.9156148927919E-038</v>
+      </c>
+      <c r="E19" s="52" t="n">
         <v>0.216477102752999</v>
       </c>
-      <c r="F19" s="61" t="n">
+      <c r="F19" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="63" t="n">
+      <c r="G19" s="53" t="n">
         <v>6.7117244842192E-013</v>
       </c>
-      <c r="H19" s="63" t="n">
+      <c r="H19" s="53" t="n">
         <v>2.50152161424738E-020</v>
       </c>
-      <c r="I19" s="63" t="n">
+      <c r="I19" s="53" t="n">
         <v>3.87086756530853E-012</v>
       </c>
-      <c r="J19" s="63" t="n">
+      <c r="J19" s="53" t="n">
         <v>2.16242021448308E-021</v>
       </c>
     </row>
@@ -6909,29 +6925,31 @@
       <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="63" t="n">
+      <c r="B20" s="53" t="n">
         <v>1.40569225114268E-022</v>
       </c>
-      <c r="C20" s="63" t="n">
+      <c r="C20" s="53" t="n">
         <v>1.71965848370678E-031</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="63" t="n">
+      <c r="D20" s="53" t="n">
+        <v>5.45548936585914E-093</v>
+      </c>
+      <c r="E20" s="53" t="n">
         <v>1.41295460619338E-016</v>
       </c>
-      <c r="F20" s="63" t="n">
+      <c r="F20" s="53" t="n">
         <v>6.7117244842192E-013</v>
       </c>
-      <c r="G20" s="61" t="n">
+      <c r="G20" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="61" t="n">
+      <c r="H20" s="52" t="n">
         <v>0.036318052440278</v>
       </c>
-      <c r="I20" s="61" t="n">
+      <c r="I20" s="52" t="n">
         <v>0.857947610497885</v>
       </c>
-      <c r="J20" s="61" t="n">
+      <c r="J20" s="52" t="n">
         <v>0.0176930992013143</v>
       </c>
     </row>
@@ -6939,29 +6957,31 @@
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="63" t="n">
+      <c r="B21" s="53" t="n">
         <v>2.44727963532734E-033</v>
       </c>
-      <c r="C21" s="63" t="n">
+      <c r="C21" s="53" t="n">
         <v>4.25216928403771E-044</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63" t="n">
+      <c r="D21" s="53" t="n">
+        <v>1.81322635172938E-114</v>
+      </c>
+      <c r="E21" s="53" t="n">
         <v>1.18149166843919E-024</v>
       </c>
-      <c r="F21" s="63" t="n">
+      <c r="F21" s="53" t="n">
         <v>2.50152161424738E-020</v>
       </c>
-      <c r="G21" s="61" t="n">
+      <c r="G21" s="52" t="n">
         <v>0.036318052440278</v>
       </c>
-      <c r="H21" s="61" t="n">
+      <c r="H21" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="61" t="n">
+      <c r="I21" s="52" t="n">
         <v>0.0251665323913943</v>
       </c>
-      <c r="J21" s="61" t="n">
+      <c r="J21" s="52" t="n">
         <v>0.77427904233013</v>
       </c>
     </row>
@@ -6969,29 +6989,31 @@
       <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="63" t="n">
+      <c r="B22" s="53" t="n">
         <v>2.30741482669337E-021</v>
       </c>
-      <c r="C22" s="63" t="n">
+      <c r="C22" s="53" t="n">
         <v>5.64415485286877E-030</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63" t="n">
+      <c r="D22" s="53" t="n">
+        <v>8.03709397994766E-090</v>
+      </c>
+      <c r="E22" s="53" t="n">
         <v>1.04626200407502E-015</v>
       </c>
-      <c r="F22" s="63" t="n">
+      <c r="F22" s="53" t="n">
         <v>3.87086756530853E-012</v>
       </c>
-      <c r="G22" s="61" t="n">
+      <c r="G22" s="52" t="n">
         <v>0.857947610497885</v>
       </c>
-      <c r="H22" s="61" t="n">
+      <c r="H22" s="52" t="n">
         <v>0.0251665323913943</v>
       </c>
-      <c r="I22" s="61" t="n">
+      <c r="I22" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="61" t="n">
+      <c r="J22" s="52" t="n">
         <v>0.0120145434024102</v>
       </c>
     </row>
@@ -6999,29 +7021,31 @@
       <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="63" t="n">
+      <c r="B23" s="53" t="n">
         <v>7.68464116569817E-035</v>
       </c>
-      <c r="C23" s="63" t="n">
+      <c r="C23" s="53" t="n">
         <v>8.08808335907419E-046</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="63" t="n">
+      <c r="D23" s="53" t="n">
+        <v>3.18649308951078E-117</v>
+      </c>
+      <c r="E23" s="53" t="n">
         <v>8.79815661908534E-026</v>
       </c>
-      <c r="F23" s="63" t="n">
+      <c r="F23" s="53" t="n">
         <v>2.16242021448308E-021</v>
       </c>
-      <c r="G23" s="61" t="n">
+      <c r="G23" s="52" t="n">
         <v>0.0176930992013143</v>
       </c>
-      <c r="H23" s="61" t="n">
+      <c r="H23" s="52" t="n">
         <v>0.77427904233013</v>
       </c>
-      <c r="I23" s="61" t="n">
+      <c r="I23" s="52" t="n">
         <v>0.0120145434024102</v>
       </c>
-      <c r="J23" s="61" t="n">
+      <c r="J23" s="52" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ttest_ind -> ttest_rel for p-values
</commit_message>
<xml_diff>
--- a/benchmarks/summary_ali.xlsx
+++ b/benchmarks/summary_ali.xlsx
@@ -152,7 +152,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,6 +195,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -308,7 +313,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,11 +486,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6332,8 +6341,8 @@
   </sheetPr>
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6400,61 +6409,61 @@
       <c r="B4" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="43" t="n">
-        <v>0.0504374219701802</v>
+      <c r="C4" s="44" t="n">
+        <v>5.23825898734213E-017</v>
       </c>
       <c r="D4" s="44" t="n">
-        <v>4.03621174251569E-040</v>
+        <v>1.82461663520532E-076</v>
       </c>
       <c r="E4" s="44" t="n">
-        <v>2.15693119619744E-032</v>
+        <v>7.04923380829012E-056</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>1.14346370107601E-028</v>
+        <v>3.48412376481279E-046</v>
       </c>
       <c r="G4" s="44" t="n">
-        <v>3.26249484643891E-006</v>
+        <v>1.13701759299585E-014</v>
       </c>
       <c r="H4" s="44" t="n">
-        <v>8.23926807833874E-012</v>
+        <v>4.57825009212676E-029</v>
       </c>
       <c r="I4" s="44" t="n">
-        <v>2.11360881771509E-006</v>
+        <v>2.18459172835406E-015</v>
       </c>
       <c r="J4" s="44" t="n">
-        <v>2.47667411384885E-011</v>
+        <v>1.32987407881408E-027</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="43" t="n">
-        <v>0.0504374219701802</v>
+      <c r="B5" s="44" t="n">
+        <v>5.23825898734213E-017</v>
       </c>
       <c r="C5" s="43" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="44" t="n">
-        <v>1.87427687363831E-029</v>
+        <v>1.27117369486306E-053</v>
       </c>
       <c r="E5" s="44" t="n">
-        <v>2.06540484386954E-025</v>
+        <v>5.90836698988952E-042</v>
       </c>
       <c r="F5" s="44" t="n">
-        <v>3.86093209646504E-022</v>
+        <v>2.92141211341293E-034</v>
       </c>
       <c r="G5" s="44" t="n">
-        <v>1.27867844911255E-010</v>
+        <v>2.54969713445701E-025</v>
       </c>
       <c r="H5" s="44" t="n">
-        <v>6.7074216897655E-018</v>
+        <v>1.03204873378565E-041</v>
       </c>
       <c r="I5" s="44" t="n">
-        <v>8.26666023713042E-011</v>
+        <v>1.22699761765446E-026</v>
       </c>
       <c r="J5" s="44" t="n">
-        <v>2.34705491716399E-017</v>
+        <v>1.57972359299791E-039</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6462,31 +6471,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="44" t="n">
-        <v>4.03621174251569E-040</v>
+        <v>1.82461663520532E-076</v>
       </c>
       <c r="C6" s="44" t="n">
-        <v>1.87427687363831E-029</v>
+        <v>1.27117369486306E-053</v>
       </c>
       <c r="D6" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="43" t="n">
-        <v>0.029068864497185</v>
-      </c>
-      <c r="F6" s="43" t="n">
-        <v>0.154207912234445</v>
+      <c r="E6" s="45" t="n">
+        <v>0.0110251646590126</v>
+      </c>
+      <c r="F6" s="45" t="n">
+        <v>0.105768519120187</v>
       </c>
       <c r="G6" s="44" t="n">
-        <v>2.0445915625115E-063</v>
+        <v>1.70701577179601E-100</v>
       </c>
       <c r="H6" s="44" t="n">
-        <v>1.96201159291058E-081</v>
+        <v>4.23391918454843E-126</v>
       </c>
       <c r="I6" s="44" t="n">
-        <v>5.83174224551E-063</v>
+        <v>9.30513626947804E-097</v>
       </c>
       <c r="J6" s="44" t="n">
-        <v>6.49055715741062E-081</v>
+        <v>2.10997919134644E-128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6494,31 +6503,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="44" t="n">
-        <v>2.15693119619744E-032</v>
+        <v>7.04923380829012E-056</v>
       </c>
       <c r="C7" s="44" t="n">
-        <v>2.06540484386954E-025</v>
-      </c>
-      <c r="D7" s="43" t="n">
-        <v>0.029068864497185</v>
+        <v>5.90836698988952E-042</v>
+      </c>
+      <c r="D7" s="45" t="n">
+        <v>0.0110251646590126</v>
       </c>
       <c r="E7" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="43" t="n">
-        <v>0.533362718697031</v>
+      <c r="F7" s="44" t="n">
+        <v>1.15820326729087E-008</v>
       </c>
       <c r="G7" s="44" t="n">
-        <v>3.62580871059107E-049</v>
+        <v>7.11462765006432E-097</v>
       </c>
       <c r="H7" s="44" t="n">
-        <v>4.04607141702362E-060</v>
+        <v>6.36253741924856E-113</v>
       </c>
       <c r="I7" s="44" t="n">
-        <v>3.41113402276447E-049</v>
+        <v>1.99493602935022E-095</v>
       </c>
       <c r="J7" s="44" t="n">
-        <v>1.54552670227266E-059</v>
+        <v>1.82349067473206E-113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6526,31 +6535,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="44" t="n">
-        <v>1.14346370107601E-028</v>
+        <v>3.48412376481279E-046</v>
       </c>
       <c r="C8" s="44" t="n">
-        <v>3.86093209646504E-022</v>
-      </c>
-      <c r="D8" s="43" t="n">
-        <v>0.154207912234445</v>
-      </c>
-      <c r="E8" s="43" t="n">
-        <v>0.533362718697031</v>
+        <v>2.92141211341293E-034</v>
+      </c>
+      <c r="D8" s="45" t="n">
+        <v>0.105768519120187</v>
+      </c>
+      <c r="E8" s="44" t="n">
+        <v>1.15820326729087E-008</v>
       </c>
       <c r="F8" s="43" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="44" t="n">
-        <v>9.33860112155806E-045</v>
+        <v>5.74319082429559E-088</v>
       </c>
       <c r="H8" s="44" t="n">
-        <v>3.35926913009405E-055</v>
+        <v>4.19002635550324E-104</v>
       </c>
       <c r="I8" s="44" t="n">
-        <v>8.19467871620724E-045</v>
+        <v>8.87346282852292E-087</v>
       </c>
       <c r="J8" s="44" t="n">
-        <v>1.27506585070311E-054</v>
+        <v>1.88681138007557E-104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6558,31 +6567,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="44" t="n">
-        <v>3.26249484643891E-006</v>
+        <v>1.13701759299585E-014</v>
       </c>
       <c r="C9" s="44" t="n">
-        <v>1.27867844911255E-010</v>
+        <v>2.54969713445701E-025</v>
       </c>
       <c r="D9" s="44" t="n">
-        <v>2.0445915625115E-063</v>
+        <v>1.70701577179601E-100</v>
       </c>
       <c r="E9" s="44" t="n">
-        <v>3.62580871059107E-049</v>
+        <v>7.11462765006432E-097</v>
       </c>
       <c r="F9" s="44" t="n">
-        <v>9.33860112155806E-045</v>
+        <v>5.74319082429559E-088</v>
       </c>
       <c r="G9" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="43" t="n">
-        <v>0.0519003229052991</v>
-      </c>
-      <c r="I9" s="43" t="n">
-        <v>0.888144633219707</v>
-      </c>
-      <c r="J9" s="43" t="n">
-        <v>0.0787686368758518</v>
+      <c r="H9" s="44" t="n">
+        <v>5.0016637457986E-014</v>
+      </c>
+      <c r="I9" s="45" t="n">
+        <v>0.27454478326037</v>
+      </c>
+      <c r="J9" s="44" t="n">
+        <v>9.40188237110572E-022</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6590,31 +6599,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="44" t="n">
-        <v>8.23926807833874E-012</v>
+        <v>4.57825009212676E-029</v>
       </c>
       <c r="C10" s="44" t="n">
-        <v>6.7074216897655E-018</v>
+        <v>1.03204873378565E-041</v>
       </c>
       <c r="D10" s="44" t="n">
-        <v>1.96201159291058E-081</v>
+        <v>4.23391918454843E-126</v>
       </c>
       <c r="E10" s="44" t="n">
-        <v>4.04607141702362E-060</v>
+        <v>6.36253741924856E-113</v>
       </c>
       <c r="F10" s="44" t="n">
-        <v>3.35926913009405E-055</v>
-      </c>
-      <c r="G10" s="43" t="n">
-        <v>0.0519003229052991</v>
+        <v>4.19002635550324E-104</v>
+      </c>
+      <c r="G10" s="44" t="n">
+        <v>5.0016637457986E-014</v>
       </c>
       <c r="H10" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="43" t="n">
-        <v>0.0757126145912473</v>
-      </c>
-      <c r="J10" s="43" t="n">
-        <v>0.837861738886887</v>
+      <c r="I10" s="44" t="n">
+        <v>1.12442535768689E-017</v>
+      </c>
+      <c r="J10" s="45" t="n">
+        <v>0.242965836229644</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,31 +6631,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="44" t="n">
-        <v>2.11360881771509E-006</v>
+        <v>2.18459172835406E-015</v>
       </c>
       <c r="C11" s="44" t="n">
-        <v>8.26666023713042E-011</v>
+        <v>1.22699761765446E-026</v>
       </c>
       <c r="D11" s="44" t="n">
-        <v>5.83174224551E-063</v>
+        <v>9.30513626947804E-097</v>
       </c>
       <c r="E11" s="44" t="n">
-        <v>3.41113402276447E-049</v>
+        <v>1.99493602935022E-095</v>
       </c>
       <c r="F11" s="44" t="n">
-        <v>8.19467871620724E-045</v>
-      </c>
-      <c r="G11" s="43" t="n">
-        <v>0.888144633219707</v>
-      </c>
-      <c r="H11" s="43" t="n">
-        <v>0.0757126145912473</v>
+        <v>8.87346282852292E-087</v>
+      </c>
+      <c r="G11" s="45" t="n">
+        <v>0.27454478326037</v>
+      </c>
+      <c r="H11" s="44" t="n">
+        <v>1.12442535768689E-017</v>
       </c>
       <c r="I11" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="43" t="n">
-        <v>0.111585255368605</v>
+      <c r="J11" s="44" t="n">
+        <v>1.66876535318788E-012</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6654,28 +6663,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="44" t="n">
-        <v>2.47667411384885E-011</v>
+        <v>1.32987407881408E-027</v>
       </c>
       <c r="C12" s="44" t="n">
-        <v>2.34705491716399E-017</v>
+        <v>1.57972359299791E-039</v>
       </c>
       <c r="D12" s="44" t="n">
-        <v>6.49055715741062E-081</v>
+        <v>2.10997919134644E-128</v>
       </c>
       <c r="E12" s="44" t="n">
-        <v>1.54552670227266E-059</v>
+        <v>1.82349067473206E-113</v>
       </c>
       <c r="F12" s="44" t="n">
-        <v>1.27506585070311E-054</v>
-      </c>
-      <c r="G12" s="43" t="n">
-        <v>0.0787686368758518</v>
-      </c>
-      <c r="H12" s="43" t="n">
-        <v>0.837861738886887</v>
-      </c>
-      <c r="I12" s="43" t="n">
-        <v>0.111585255368605</v>
+        <v>1.88681138007557E-104</v>
+      </c>
+      <c r="G12" s="44" t="n">
+        <v>9.40188237110572E-022</v>
+      </c>
+      <c r="H12" s="45" t="n">
+        <v>0.242965836229644</v>
+      </c>
+      <c r="I12" s="44" t="n">
+        <v>1.66876535318788E-012</v>
       </c>
       <c r="J12" s="43" t="n">
         <v>1</v>
@@ -6732,282 +6741,282 @@
       <c r="B15" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="43" t="n">
-        <v>0.0464204936614076</v>
-      </c>
-      <c r="D15" s="43" t="n">
-        <v>1.11886995766341E-029</v>
-      </c>
-      <c r="E15" s="43" t="n">
-        <v>0.430766044004024</v>
-      </c>
-      <c r="F15" s="43" t="n">
-        <v>0.0337628569558176</v>
-      </c>
-      <c r="G15" s="43" t="n">
-        <v>1.18043158517604E-022</v>
-      </c>
-      <c r="H15" s="43" t="n">
-        <v>9.60579473938845E-034</v>
-      </c>
-      <c r="I15" s="43" t="n">
-        <v>5.99003926061061E-023</v>
-      </c>
-      <c r="J15" s="43" t="n">
-        <v>1.0696537483824E-033</v>
+      <c r="C15" s="44" t="n">
+        <v>1.20538010782463E-042</v>
+      </c>
+      <c r="D15" s="44" t="n">
+        <v>9.78720764887794E-046</v>
+      </c>
+      <c r="E15" s="45" t="n">
+        <v>0.120649633734279</v>
+      </c>
+      <c r="F15" s="44" t="n">
+        <v>0.000675801840840618</v>
+      </c>
+      <c r="G15" s="44" t="n">
+        <v>9.36602308018282E-044</v>
+      </c>
+      <c r="H15" s="44" t="n">
+        <v>7.49670320257962E-061</v>
+      </c>
+      <c r="I15" s="44" t="n">
+        <v>9.7030303128131E-048</v>
+      </c>
+      <c r="J15" s="44" t="n">
+        <v>1.99635132806869E-056</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="43" t="n">
-        <v>0.0464204936614076</v>
+      <c r="B16" s="44" t="n">
+        <v>1.20538010782463E-042</v>
       </c>
       <c r="C16" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="43" t="n">
-        <v>6.69869287499587E-021</v>
-      </c>
-      <c r="E16" s="43" t="n">
-        <v>0.00807972941599414</v>
-      </c>
-      <c r="F16" s="43" t="n">
-        <v>5.89302677569622E-005</v>
-      </c>
-      <c r="G16" s="43" t="n">
-        <v>1.39146979587666E-031</v>
-      </c>
-      <c r="H16" s="43" t="n">
-        <v>1.31533356408265E-044</v>
-      </c>
-      <c r="I16" s="43" t="n">
-        <v>6.70472815605871E-032</v>
-      </c>
-      <c r="J16" s="43" t="n">
-        <v>1.57420764119522E-044</v>
+      <c r="D16" s="44" t="n">
+        <v>7.58051898648505E-033</v>
+      </c>
+      <c r="E16" s="44" t="n">
+        <v>4.2364928625964E-007</v>
+      </c>
+      <c r="F16" s="44" t="n">
+        <v>2.49238838945545E-010</v>
+      </c>
+      <c r="G16" s="44" t="n">
+        <v>1.2273033469118E-057</v>
+      </c>
+      <c r="H16" s="44" t="n">
+        <v>2.7996235786395E-076</v>
+      </c>
+      <c r="I16" s="44" t="n">
+        <v>3.41568846637369E-062</v>
+      </c>
+      <c r="J16" s="44" t="n">
+        <v>2.51954361903932E-071</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="43" t="n">
-        <v>1.11886995766341E-029</v>
-      </c>
-      <c r="C17" s="43" t="n">
-        <v>6.69869287499587E-021</v>
+      <c r="B17" s="44" t="n">
+        <v>9.78720764887794E-046</v>
+      </c>
+      <c r="C17" s="44" t="n">
+        <v>7.58051898648505E-033</v>
       </c>
       <c r="D17" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="43" t="n">
-        <v>5.04952182463349E-030</v>
-      </c>
-      <c r="F17" s="43" t="n">
-        <v>6.9156148927919E-038</v>
-      </c>
-      <c r="G17" s="43" t="n">
-        <v>3.65677054746204E-093</v>
-      </c>
-      <c r="H17" s="43" t="n">
-        <v>1.34412058108108E-115</v>
-      </c>
-      <c r="I17" s="43" t="n">
-        <v>1.80577109806434E-093</v>
-      </c>
-      <c r="J17" s="43" t="n">
-        <v>2.6755955987647E-115</v>
+      <c r="E17" s="44" t="n">
+        <v>2.43321831943305E-033</v>
+      </c>
+      <c r="F17" s="44" t="n">
+        <v>1.50184609697506E-036</v>
+      </c>
+      <c r="G17" s="44" t="n">
+        <v>4.89118697426647E-119</v>
+      </c>
+      <c r="H17" s="44" t="n">
+        <v>2.6833524635436E-141</v>
+      </c>
+      <c r="I17" s="44" t="n">
+        <v>2.75709204212942E-117</v>
+      </c>
+      <c r="J17" s="44" t="n">
+        <v>6.04327951652978E-143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="43" t="n">
-        <v>0.430766044004024</v>
-      </c>
-      <c r="C18" s="43" t="n">
-        <v>0.00807972941599414</v>
-      </c>
-      <c r="D18" s="43" t="n">
-        <v>5.04952182463349E-030</v>
+      <c r="B18" s="45" t="n">
+        <v>0.120649633734279</v>
+      </c>
+      <c r="C18" s="44" t="n">
+        <v>4.2364928625964E-007</v>
+      </c>
+      <c r="D18" s="44" t="n">
+        <v>2.43321831943305E-033</v>
       </c>
       <c r="E18" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="43" t="n">
-        <v>0.216477102752999</v>
-      </c>
-      <c r="G18" s="43" t="n">
-        <v>1.24165278499916E-016</v>
-      </c>
-      <c r="H18" s="43" t="n">
-        <v>6.53990556435391E-025</v>
-      </c>
-      <c r="I18" s="43" t="n">
-        <v>6.96113433443905E-017</v>
-      </c>
-      <c r="J18" s="43" t="n">
-        <v>6.66431512707055E-025</v>
+      <c r="F18" s="44" t="n">
+        <v>1.63614606587605E-007</v>
+      </c>
+      <c r="G18" s="44" t="n">
+        <v>3.05492666745932E-036</v>
+      </c>
+      <c r="H18" s="44" t="n">
+        <v>3.47870045492453E-049</v>
+      </c>
+      <c r="I18" s="44" t="n">
+        <v>6.11455441871149E-038</v>
+      </c>
+      <c r="J18" s="44" t="n">
+        <v>6.00533067144299E-047</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="43" t="n">
-        <v>0.0337628569558176</v>
-      </c>
-      <c r="C19" s="43" t="n">
-        <v>5.89302677569622E-005</v>
-      </c>
-      <c r="D19" s="43" t="n">
-        <v>6.9156148927919E-038</v>
-      </c>
-      <c r="E19" s="43" t="n">
-        <v>0.216477102752999</v>
+      <c r="B19" s="44" t="n">
+        <v>0.000675801840840618</v>
+      </c>
+      <c r="C19" s="44" t="n">
+        <v>2.49238838945545E-010</v>
+      </c>
+      <c r="D19" s="44" t="n">
+        <v>1.50184609697506E-036</v>
+      </c>
+      <c r="E19" s="44" t="n">
+        <v>1.63614606587605E-007</v>
       </c>
       <c r="F19" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="43" t="n">
-        <v>5.98151218678731E-013</v>
-      </c>
-      <c r="H19" s="43" t="n">
-        <v>1.46978723958007E-020</v>
-      </c>
-      <c r="I19" s="43" t="n">
-        <v>3.47557018276505E-013</v>
-      </c>
-      <c r="J19" s="43" t="n">
-        <v>1.47568670030489E-020</v>
+      <c r="G19" s="44" t="n">
+        <v>5.00711136711025E-027</v>
+      </c>
+      <c r="H19" s="44" t="n">
+        <v>3.07014577124314E-040</v>
+      </c>
+      <c r="I19" s="44" t="n">
+        <v>1.50257009411195E-028</v>
+      </c>
+      <c r="J19" s="44" t="n">
+        <v>4.90669040394034E-038</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="43" t="n">
-        <v>1.18043158517604E-022</v>
-      </c>
-      <c r="C20" s="43" t="n">
-        <v>1.39146979587666E-031</v>
-      </c>
-      <c r="D20" s="43" t="n">
-        <v>3.65677054746204E-093</v>
-      </c>
-      <c r="E20" s="43" t="n">
-        <v>1.24165278499916E-016</v>
-      </c>
-      <c r="F20" s="43" t="n">
-        <v>5.98151218678731E-013</v>
+      <c r="B20" s="44" t="n">
+        <v>9.36602308018282E-044</v>
+      </c>
+      <c r="C20" s="44" t="n">
+        <v>1.2273033469118E-057</v>
+      </c>
+      <c r="D20" s="44" t="n">
+        <v>4.89118697426647E-119</v>
+      </c>
+      <c r="E20" s="44" t="n">
+        <v>3.05492666745932E-036</v>
+      </c>
+      <c r="F20" s="44" t="n">
+        <v>5.00711136711025E-027</v>
       </c>
       <c r="G20" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="43" t="n">
-        <v>0.0353709553672543</v>
-      </c>
-      <c r="I20" s="43" t="n">
-        <v>0.914142630099924</v>
-      </c>
-      <c r="J20" s="43" t="n">
-        <v>0.0336502646012091</v>
+      <c r="H20" s="44" t="n">
+        <v>2.33024034628679E-015</v>
+      </c>
+      <c r="I20" s="45" t="n">
+        <v>0.294111540408825</v>
+      </c>
+      <c r="J20" s="44" t="n">
+        <v>7.12550125144987E-018</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="43" t="n">
-        <v>9.60579473938845E-034</v>
-      </c>
-      <c r="C21" s="43" t="n">
-        <v>1.31533356408265E-044</v>
-      </c>
-      <c r="D21" s="43" t="n">
-        <v>1.34412058108108E-115</v>
-      </c>
-      <c r="E21" s="43" t="n">
-        <v>6.53990556435391E-025</v>
-      </c>
-      <c r="F21" s="43" t="n">
-        <v>1.46978723958007E-020</v>
-      </c>
-      <c r="G21" s="43" t="n">
-        <v>0.0353709553672543</v>
+      <c r="B21" s="44" t="n">
+        <v>7.49670320257962E-061</v>
+      </c>
+      <c r="C21" s="44" t="n">
+        <v>2.7996235786395E-076</v>
+      </c>
+      <c r="D21" s="44" t="n">
+        <v>2.6833524635436E-141</v>
+      </c>
+      <c r="E21" s="44" t="n">
+        <v>3.47870045492453E-049</v>
+      </c>
+      <c r="F21" s="44" t="n">
+        <v>3.07014577124314E-040</v>
+      </c>
+      <c r="G21" s="44" t="n">
+        <v>2.33024034628679E-015</v>
       </c>
       <c r="H21" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="43" t="n">
-        <v>0.0478025494223026</v>
-      </c>
-      <c r="J21" s="43" t="n">
-        <v>0.974932602406227</v>
+      <c r="I21" s="44" t="n">
+        <v>1.16454799322193E-014</v>
+      </c>
+      <c r="J21" s="45" t="n">
+        <v>0.814915424620923</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="43" t="n">
-        <v>5.99003926061061E-023</v>
-      </c>
-      <c r="C22" s="43" t="n">
-        <v>6.70472815605871E-032</v>
-      </c>
-      <c r="D22" s="43" t="n">
-        <v>1.80577109806434E-093</v>
-      </c>
-      <c r="E22" s="43" t="n">
-        <v>6.96113433443905E-017</v>
-      </c>
-      <c r="F22" s="43" t="n">
-        <v>3.47557018276505E-013</v>
-      </c>
-      <c r="G22" s="43" t="n">
-        <v>0.914142630099924</v>
-      </c>
-      <c r="H22" s="43" t="n">
-        <v>0.0478025494223026</v>
+      <c r="B22" s="44" t="n">
+        <v>9.7030303128131E-048</v>
+      </c>
+      <c r="C22" s="44" t="n">
+        <v>3.41568846637369E-062</v>
+      </c>
+      <c r="D22" s="44" t="n">
+        <v>2.75709204212942E-117</v>
+      </c>
+      <c r="E22" s="44" t="n">
+        <v>6.11455441871149E-038</v>
+      </c>
+      <c r="F22" s="44" t="n">
+        <v>1.50257009411195E-028</v>
+      </c>
+      <c r="G22" s="45" t="n">
+        <v>0.294111540408825</v>
+      </c>
+      <c r="H22" s="44" t="n">
+        <v>1.16454799322193E-014</v>
       </c>
       <c r="I22" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="43" t="n">
-        <v>0.0455330572680915</v>
+      <c r="J22" s="44" t="n">
+        <v>2.50769683804307E-012</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="43" t="n">
-        <v>1.0696537483824E-033</v>
-      </c>
-      <c r="C23" s="43" t="n">
-        <v>1.57420764119522E-044</v>
-      </c>
-      <c r="D23" s="43" t="n">
-        <v>2.6755955987647E-115</v>
-      </c>
-      <c r="E23" s="43" t="n">
-        <v>6.66431512707055E-025</v>
-      </c>
-      <c r="F23" s="43" t="n">
-        <v>1.47568670030489E-020</v>
-      </c>
-      <c r="G23" s="43" t="n">
-        <v>0.0336502646012091</v>
-      </c>
-      <c r="H23" s="43" t="n">
-        <v>0.974932602406227</v>
-      </c>
-      <c r="I23" s="43" t="n">
-        <v>0.0455330572680915</v>
+      <c r="B23" s="44" t="n">
+        <v>1.99635132806869E-056</v>
+      </c>
+      <c r="C23" s="44" t="n">
+        <v>2.51954361903932E-071</v>
+      </c>
+      <c r="D23" s="44" t="n">
+        <v>6.04327951652978E-143</v>
+      </c>
+      <c r="E23" s="44" t="n">
+        <v>6.00533067144299E-047</v>
+      </c>
+      <c r="F23" s="44" t="n">
+        <v>4.90669040394034E-038</v>
+      </c>
+      <c r="G23" s="44" t="n">
+        <v>7.12550125144987E-018</v>
+      </c>
+      <c r="H23" s="45" t="n">
+        <v>0.814915424620923</v>
+      </c>
+      <c r="I23" s="44" t="n">
+        <v>2.50769683804307E-012</v>
       </c>
       <c r="J23" s="43" t="n">
         <v>1</v>

</xml_diff>